<commit_message>
Data update, 8/4 and 8/8/22 runs.
</commit_message>
<xml_diff>
--- a/analysis/resources/WaTCH_Tables.xlsx
+++ b/analysis/resources/WaTCH_Tables.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tpd0001/Dropbox (DriscollMML)/Project_WaTCH/ANALYSIS/RESOURCES/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tpd0001/github/watch-wv/analysis/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04737A98-472E-3E43-90F5-8BE41072C42A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1E65D25-4843-D948-A603-E747B96377CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="600" yWindow="500" windowWidth="26960" windowHeight="20500" xr2:uid="{ABEE2980-A2EF-284E-9534-8BF6C1D1D8CC}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="804" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="814" uniqueCount="233">
   <si>
     <t>capacity_mgd</t>
   </si>
@@ -724,6 +724,15 @@
   </si>
   <si>
     <t>Cabell,Wayne</t>
+  </si>
+  <si>
+    <t>PointPleasantWWTP-01</t>
+  </si>
+  <si>
+    <t>Mason</t>
+  </si>
+  <si>
+    <t>Point Pleasant</t>
   </si>
 </sst>
 </file>
@@ -1290,13 +1299,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0856F7A-D0C0-3942-9027-9FB2F3C2C3E0}">
-  <dimension ref="A1:R72"/>
+  <dimension ref="A1:R73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="F34" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B52" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K60" sqref="K60"/>
+      <selection pane="bottomRight" activeCell="N74" sqref="N74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5114,6 +5123,7 @@
       <c r="G72" s="4" t="s">
         <v>182</v>
       </c>
+      <c r="J72" s="21"/>
       <c r="K72" s="32" t="s">
         <v>194</v>
       </c>
@@ -5126,6 +5136,53 @@
         <v>31</v>
       </c>
       <c r="Q72" s="33"/>
+    </row>
+    <row r="73" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A73" s="21" t="s">
+        <v>230</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C73" s="21" t="s">
+        <v>232</v>
+      </c>
+      <c r="D73" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="E73" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="F73" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="G73" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="H73">
+        <v>-82.135114799999997</v>
+      </c>
+      <c r="I73">
+        <v>38.856708400000002</v>
+      </c>
+      <c r="J73" s="21" t="s">
+        <v>230</v>
+      </c>
+      <c r="K73" s="21" t="s">
+        <v>231</v>
+      </c>
+      <c r="L73" s="18">
+        <v>0.7</v>
+      </c>
+      <c r="M73" s="15">
+        <v>5515</v>
+      </c>
+      <c r="N73" s="18">
+        <v>26700</v>
+      </c>
+      <c r="O73" s="36" t="s">
+        <v>18</v>
+      </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:R58">

</xml_diff>

<commit_message>
Data update 9/8 and 9/9.
</commit_message>
<xml_diff>
--- a/analysis/resources/WaTCH_Tables.xlsx
+++ b/analysis/resources/WaTCH_Tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tpd0001/github/watch-wv/analysis/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6FEA50F-D29F-F645-9CA3-D6402CFA389C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B23D7CC-3944-F04A-843D-331D32BDCB8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="600" yWindow="500" windowWidth="26960" windowHeight="20500" xr2:uid="{ABEE2980-A2EF-284E-9534-8BF6C1D1D8CC}"/>
   </bookViews>
@@ -1330,7 +1330,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C14" sqref="C14"/>
+      <selection pane="bottomRight" activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2447,7 +2447,7 @@
         <v>73</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>122</v>
+        <v>78</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>98</v>

</xml_diff>

<commit_message>
Data update 9/16 and push to dashboard. Huntington removed from display pending data integration with MU.
</commit_message>
<xml_diff>
--- a/analysis/resources/WaTCH_Tables.xlsx
+++ b/analysis/resources/WaTCH_Tables.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tpd0001/github/watch-wv/analysis/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B23D7CC-3944-F04A-843D-331D32BDCB8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A7314C3-D212-C347-A89D-B7C637AA797D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="600" yWindow="500" windowWidth="26960" windowHeight="20500" xr2:uid="{ABEE2980-A2EF-284E-9534-8BF6C1D1D8CC}"/>
   </bookViews>
@@ -1327,10 +1327,10 @@
   <dimension ref="A1:R74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B36" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B23" sqref="B23"/>
+      <selection pane="bottomRight" activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3419,7 +3419,7 @@
         <v>207</v>
       </c>
       <c r="B40" s="33" t="s">
-        <v>122</v>
+        <v>78</v>
       </c>
       <c r="C40" s="32" t="s">
         <v>190</v>

</xml_diff>

<commit_message>
Data update 1/6/23. Also fixed error in NWSS merge to take care of empty rows. Not fully debugged yet.
</commit_message>
<xml_diff>
--- a/analysis/resources/WaTCH_Tables.xlsx
+++ b/analysis/resources/WaTCH_Tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tpd0001/github/watch-wv/analysis/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A7314C3-D212-C347-A89D-B7C637AA797D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49956801-D481-F444-96D6-4EB217BE7678}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="500" windowWidth="26960" windowHeight="20500" xr2:uid="{ABEE2980-A2EF-284E-9534-8BF6C1D1D8CC}"/>
+    <workbookView xWindow="600" yWindow="760" windowWidth="26960" windowHeight="18880" xr2:uid="{ABEE2980-A2EF-284E-9534-8BF6C1D1D8CC}"/>
   </bookViews>
   <sheets>
     <sheet name="locations" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="826" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="829" uniqueCount="236">
   <si>
     <t>capacity_mgd</t>
   </si>
@@ -920,7 +920,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -958,7 +958,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -994,7 +993,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1028,7 +1026,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1316,7 +1314,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1327,10 +1325,10 @@
   <dimension ref="A1:R74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B36" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="M19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B41" sqref="B41"/>
+      <selection pane="bottomRight" activeCell="Q49" sqref="Q49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1377,7 +1375,7 @@
       <c r="H1" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="I1" s="26" t="s">
+      <c r="I1" s="25" t="s">
         <v>152</v>
       </c>
       <c r="J1" s="1" t="s">
@@ -1409,7 +1407,7 @@
       </c>
     </row>
     <row r="2" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="21" t="s">
+      <c r="A2" t="s">
         <v>125</v>
       </c>
       <c r="B2" s="6" t="s">
@@ -1459,7 +1457,7 @@
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="41" t="s">
         <v>34</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -1515,7 +1513,7 @@
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A4" s="43" t="s">
+      <c r="A4" s="41" t="s">
         <v>44</v>
       </c>
       <c r="B4" s="6" t="s">
@@ -1571,7 +1569,7 @@
       </c>
     </row>
     <row r="5" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="43" t="s">
+      <c r="A5" s="41" t="s">
         <v>35</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -1627,7 +1625,7 @@
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A6" s="43" t="s">
+      <c r="A6" s="41" t="s">
         <v>36</v>
       </c>
       <c r="B6" s="6" t="s">
@@ -1683,7 +1681,7 @@
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A7" s="43" t="s">
+      <c r="A7" s="41" t="s">
         <v>231</v>
       </c>
       <c r="B7" s="6" t="s">
@@ -1739,7 +1737,7 @@
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A8" s="43" t="s">
+      <c r="A8" s="41" t="s">
         <v>45</v>
       </c>
       <c r="B8" s="6" t="s">
@@ -1795,19 +1793,19 @@
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A9" s="27" t="s">
+      <c r="A9" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="B9" s="28" t="s">
+      <c r="B9" s="27" t="s">
         <v>148</v>
       </c>
-      <c r="C9" s="27" t="s">
+      <c r="C9" s="26" t="s">
         <v>105</v>
       </c>
-      <c r="D9" s="27" t="s">
+      <c r="D9" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="E9" s="27" t="s">
+      <c r="E9" s="26" t="s">
         <v>76</v>
       </c>
       <c r="F9" s="4" t="s">
@@ -1816,49 +1814,49 @@
       <c r="G9" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="H9" s="27">
+      <c r="H9" s="26">
         <v>-78.98272</v>
       </c>
-      <c r="I9" s="29">
+      <c r="I9" s="28">
         <v>39.438070000000003</v>
       </c>
-      <c r="J9" s="27" t="s">
+      <c r="J9" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="K9" s="27" t="s">
+      <c r="K9" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="L9" s="30">
+      <c r="L9" s="29">
         <v>-1</v>
       </c>
-      <c r="M9" s="30">
+      <c r="M9" s="29">
         <v>1193</v>
       </c>
-      <c r="N9" s="31">
+      <c r="N9" s="30">
         <v>26868</v>
       </c>
-      <c r="O9" s="27" t="s">
+      <c r="O9" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="P9" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q9" s="28">
+      <c r="P9" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q9" s="27">
         <v>26726</v>
       </c>
       <c r="R9" s="4"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A10" s="43" t="s">
+      <c r="A10" s="41" t="s">
         <v>217</v>
       </c>
-      <c r="B10" s="33" t="s">
+      <c r="B10" s="32" t="s">
         <v>78</v>
       </c>
-      <c r="C10" s="32" t="s">
+      <c r="C10" s="31" t="s">
         <v>218</v>
       </c>
-      <c r="D10" s="32" t="s">
+      <c r="D10" s="31" t="s">
         <v>27</v>
       </c>
       <c r="E10" s="4" t="s">
@@ -1870,21 +1868,21 @@
       <c r="G10" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="K10" s="32" t="s">
+      <c r="K10" s="31" t="s">
         <v>192</v>
       </c>
-      <c r="L10" s="35"/>
-      <c r="M10" s="35"/>
-      <c r="N10" s="42">
+      <c r="L10" s="34"/>
+      <c r="M10" s="34"/>
+      <c r="N10" s="40">
         <v>96319</v>
       </c>
-      <c r="P10" s="34" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q10" s="33"/>
+      <c r="P10" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q10" s="32"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A11" s="43" t="s">
+      <c r="A11" s="41" t="s">
         <v>32</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -1940,16 +1938,16 @@
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A12" s="43" t="s">
+      <c r="A12" s="41" t="s">
         <v>223</v>
       </c>
-      <c r="B12" s="33" t="s">
+      <c r="B12" s="32" t="s">
         <v>78</v>
       </c>
-      <c r="C12" s="32" t="s">
+      <c r="C12" s="31" t="s">
         <v>224</v>
       </c>
-      <c r="D12" s="32" t="s">
+      <c r="D12" s="31" t="s">
         <v>27</v>
       </c>
       <c r="E12" s="4" t="s">
@@ -1961,22 +1959,21 @@
       <c r="G12" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="J12" s="21"/>
-      <c r="K12" s="32" t="s">
+      <c r="K12" s="31" t="s">
         <v>192</v>
       </c>
-      <c r="L12" s="35"/>
-      <c r="M12" s="35"/>
-      <c r="N12" s="42">
+      <c r="L12" s="34"/>
+      <c r="M12" s="34"/>
+      <c r="N12" s="40">
         <v>96319</v>
       </c>
-      <c r="P12" s="34" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q12" s="33"/>
+      <c r="P12" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q12" s="32"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A13" s="43" t="s">
+      <c r="A13" s="41" t="s">
         <v>38</v>
       </c>
       <c r="B13" s="6" t="s">
@@ -2032,7 +2029,7 @@
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A14" s="43" t="s">
+      <c r="A14" s="41" t="s">
         <v>39</v>
       </c>
       <c r="B14" s="6" t="s">
@@ -2088,7 +2085,7 @@
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A15" s="43" t="s">
+      <c r="A15" s="41" t="s">
         <v>40</v>
       </c>
       <c r="B15" s="6" t="s">
@@ -2144,7 +2141,7 @@
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A16" s="43" t="s">
+      <c r="A16" s="41" t="s">
         <v>41</v>
       </c>
       <c r="B16" s="6" t="s">
@@ -2200,7 +2197,7 @@
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A17" s="43" t="s">
+      <c r="A17" s="41" t="s">
         <v>42</v>
       </c>
       <c r="B17" s="6" t="s">
@@ -2256,7 +2253,7 @@
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A18" s="43" t="s">
+      <c r="A18" s="41" t="s">
         <v>43</v>
       </c>
       <c r="B18" s="6" t="s">
@@ -2312,16 +2309,16 @@
       </c>
     </row>
     <row r="19" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="43" t="s">
+      <c r="A19" s="41" t="s">
         <v>219</v>
       </c>
-      <c r="B19" s="33" t="s">
+      <c r="B19" s="32" t="s">
         <v>78</v>
       </c>
-      <c r="C19" s="32" t="s">
+      <c r="C19" s="31" t="s">
         <v>220</v>
       </c>
-      <c r="D19" s="32" t="s">
+      <c r="D19" s="31" t="s">
         <v>27</v>
       </c>
       <c r="E19" s="4" t="s">
@@ -2336,32 +2333,32 @@
       <c r="H19"/>
       <c r="I19"/>
       <c r="J19"/>
-      <c r="K19" s="32" t="s">
+      <c r="K19" s="31" t="s">
         <v>192</v>
       </c>
-      <c r="L19" s="35"/>
-      <c r="M19" s="35"/>
-      <c r="N19" s="42">
+      <c r="L19" s="34"/>
+      <c r="M19" s="34"/>
+      <c r="N19" s="40">
         <v>96319</v>
       </c>
       <c r="O19"/>
-      <c r="P19" s="34" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q19" s="33"/>
+      <c r="P19" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q19" s="32"/>
       <c r="R19"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A20" s="43" t="s">
+      <c r="A20" s="41" t="s">
         <v>221</v>
       </c>
-      <c r="B20" s="33" t="s">
+      <c r="B20" s="32" t="s">
         <v>78</v>
       </c>
-      <c r="C20" s="32" t="s">
+      <c r="C20" s="31" t="s">
         <v>222</v>
       </c>
-      <c r="D20" s="32" t="s">
+      <c r="D20" s="31" t="s">
         <v>27</v>
       </c>
       <c r="E20" s="4" t="s">
@@ -2373,21 +2370,21 @@
       <c r="G20" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="K20" s="32" t="s">
+      <c r="K20" s="31" t="s">
         <v>192</v>
       </c>
-      <c r="L20" s="35"/>
-      <c r="M20" s="35"/>
-      <c r="N20" s="42">
+      <c r="L20" s="34"/>
+      <c r="M20" s="34"/>
+      <c r="N20" s="40">
         <v>96319</v>
       </c>
-      <c r="P20" s="34" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q20" s="33"/>
+      <c r="P20" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q20" s="32"/>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A21" s="43" t="s">
+      <c r="A21" s="41" t="s">
         <v>46</v>
       </c>
       <c r="B21" s="6" t="s">
@@ -2443,7 +2440,7 @@
       </c>
     </row>
     <row r="22" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="44" t="s">
+      <c r="A22" s="42" t="s">
         <v>73</v>
       </c>
       <c r="B22" s="3" t="s">
@@ -2497,7 +2494,7 @@
       <c r="R22"/>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A23" s="44" t="s">
+      <c r="A23" s="42" t="s">
         <v>49</v>
       </c>
       <c r="B23" s="6" t="s">
@@ -2551,7 +2548,7 @@
       <c r="R23" s="4"/>
     </row>
     <row r="24" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="44" t="s">
+      <c r="A24" s="42" t="s">
         <v>54</v>
       </c>
       <c r="B24" s="6" t="s">
@@ -2604,7 +2601,7 @@
       </c>
     </row>
     <row r="25" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="44" t="s">
+      <c r="A25" s="42" t="s">
         <v>52</v>
       </c>
       <c r="B25" s="3" t="s">
@@ -2658,7 +2655,7 @@
       <c r="R25"/>
     </row>
     <row r="26" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="44" t="s">
+      <c r="A26" s="42" t="s">
         <v>53</v>
       </c>
       <c r="B26" s="3" t="s">
@@ -2712,7 +2709,7 @@
       <c r="R26"/>
     </row>
     <row r="27" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="44" t="s">
+      <c r="A27" s="42" t="s">
         <v>50</v>
       </c>
       <c r="B27" s="3" t="s">
@@ -2766,7 +2763,7 @@
       <c r="R27" s="4"/>
     </row>
     <row r="28" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="44" t="s">
+      <c r="A28" s="42" t="s">
         <v>51</v>
       </c>
       <c r="B28" s="6" t="s">
@@ -2874,7 +2871,7 @@
       </c>
       <c r="R29" s="4"/>
     </row>
-    <row r="30" spans="1:18" s="38" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:18" s="37" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="19" t="s">
         <v>23</v>
       </c>
@@ -2968,7 +2965,7 @@
       <c r="M31" s="15">
         <v>50000</v>
       </c>
-      <c r="N31" s="42">
+      <c r="N31" s="40">
         <v>183279</v>
       </c>
       <c r="O31" t="s">
@@ -3418,53 +3415,53 @@
       <c r="A40" s="19" t="s">
         <v>207</v>
       </c>
-      <c r="B40" s="33" t="s">
+      <c r="B40" s="32" t="s">
         <v>78</v>
       </c>
-      <c r="C40" s="32" t="s">
+      <c r="C40" s="31" t="s">
         <v>190</v>
       </c>
-      <c r="D40" s="34" t="s">
+      <c r="D40" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="E40" s="34" t="s">
+      <c r="E40" s="33" t="s">
         <v>75</v>
       </c>
-      <c r="F40" s="34" t="s">
-        <v>178</v>
-      </c>
-      <c r="G40" s="34" t="s">
-        <v>178</v>
-      </c>
-      <c r="H40" s="32">
+      <c r="F40" s="33" t="s">
+        <v>178</v>
+      </c>
+      <c r="G40" s="33" t="s">
+        <v>178</v>
+      </c>
+      <c r="H40" s="31">
         <v>-82.528864034905197</v>
       </c>
-      <c r="I40" s="32">
+      <c r="I40" s="31">
         <v>38.400744931017101</v>
       </c>
-      <c r="J40" s="21" t="s">
+      <c r="J40" t="s">
         <v>207</v>
       </c>
-      <c r="K40" s="32" t="s">
+      <c r="K40" s="31" t="s">
         <v>227</v>
       </c>
-      <c r="L40" s="35">
+      <c r="L40" s="34">
         <v>17</v>
       </c>
-      <c r="M40" s="35">
+      <c r="M40" s="34">
         <v>56000</v>
       </c>
-      <c r="N40" s="42">
+      <c r="N40" s="40">
         <f>96319+42481</f>
         <v>138800</v>
       </c>
-      <c r="O40" s="36" t="s">
+      <c r="O40" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="P40" s="34" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q40" s="37">
+      <c r="P40" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q40" s="36">
         <v>25704</v>
       </c>
       <c r="R40"/>
@@ -3854,10 +3851,10 @@
       <c r="B48" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="C48" s="21" t="s">
+      <c r="C48" t="s">
         <v>230</v>
       </c>
-      <c r="D48" s="34" t="s">
+      <c r="D48" s="33" t="s">
         <v>26</v>
       </c>
       <c r="E48" s="4" t="s">
@@ -3875,10 +3872,10 @@
       <c r="I48">
         <v>38.856708400000002</v>
       </c>
-      <c r="J48" s="21" t="s">
+      <c r="J48" t="s">
         <v>228</v>
       </c>
-      <c r="K48" s="21" t="s">
+      <c r="K48" t="s">
         <v>229</v>
       </c>
       <c r="L48" s="18">
@@ -3890,11 +3887,15 @@
       <c r="N48" s="18">
         <v>26700</v>
       </c>
-      <c r="O48" s="36" t="s">
+      <c r="O48" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="P48"/>
-      <c r="Q48" s="3"/>
+      <c r="P48" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q48" s="3">
+        <v>25550</v>
+      </c>
       <c r="R48"/>
     </row>
     <row r="49" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -4276,7 +4277,7 @@
       <c r="A56" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="B56" s="22" t="s">
+      <c r="B56" s="21" t="s">
         <v>148</v>
       </c>
       <c r="C56" s="20" t="s">
@@ -4306,13 +4307,13 @@
       <c r="K56" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="L56" s="24">
+      <c r="L56" s="23">
         <v>1.8</v>
       </c>
-      <c r="M56" s="25">
+      <c r="M56" s="24">
         <v>3255</v>
       </c>
-      <c r="N56" s="25">
+      <c r="N56" s="24">
         <v>17884</v>
       </c>
       <c r="O56" s="20" t="s">
@@ -4321,7 +4322,7 @@
       <c r="P56" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="Q56" s="22">
+      <c r="Q56" s="21">
         <v>25411</v>
       </c>
       <c r="R56" s="20"/>
@@ -4330,7 +4331,7 @@
       <c r="A57" s="20" t="s">
         <v>147</v>
       </c>
-      <c r="B57" s="22" t="s">
+      <c r="B57" s="21" t="s">
         <v>148</v>
       </c>
       <c r="C57" s="20" t="s">
@@ -4356,72 +4357,74 @@
       <c r="K57" s="20" t="s">
         <v>142</v>
       </c>
-      <c r="L57" s="24">
+      <c r="L57" s="23">
         <v>4</v>
       </c>
-      <c r="M57" s="25">
+      <c r="M57" s="24">
         <v>20411</v>
       </c>
       <c r="N57" s="16">
         <v>21939</v>
       </c>
       <c r="O57" s="20"/>
-      <c r="P57" s="20"/>
-      <c r="Q57" s="22"/>
+      <c r="P57" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q57" s="21"/>
     </row>
     <row r="58" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A58" s="19" t="s">
         <v>209</v>
       </c>
-      <c r="B58" s="33" t="s">
+      <c r="B58" s="32" t="s">
         <v>78</v>
       </c>
-      <c r="C58" s="32" t="s">
+      <c r="C58" s="31" t="s">
         <v>191</v>
       </c>
-      <c r="D58" s="34" t="s">
+      <c r="D58" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="E58" s="34" t="s">
+      <c r="E58" s="33" t="s">
         <v>75</v>
       </c>
-      <c r="F58" s="34" t="s">
-        <v>178</v>
-      </c>
-      <c r="G58" s="34" t="s">
-        <v>178</v>
-      </c>
-      <c r="H58" s="32">
+      <c r="F58" s="33" t="s">
+        <v>178</v>
+      </c>
+      <c r="G58" s="33" t="s">
+        <v>178</v>
+      </c>
+      <c r="H58" s="31">
         <v>-82.285698770801503</v>
       </c>
-      <c r="I58" s="32">
+      <c r="I58" s="31">
         <v>38.414946823509098</v>
       </c>
-      <c r="J58" s="21" t="s">
+      <c r="J58" t="s">
         <v>209</v>
       </c>
-      <c r="K58" s="32" t="s">
+      <c r="K58" s="31" t="s">
         <v>192</v>
       </c>
-      <c r="L58" s="35">
+      <c r="L58" s="34">
         <v>1.8</v>
       </c>
-      <c r="M58" s="35">
+      <c r="M58" s="34">
         <v>4000</v>
       </c>
-      <c r="N58" s="42">
+      <c r="N58" s="40">
         <v>96319</v>
       </c>
-      <c r="O58" s="32" t="s">
+      <c r="O58" s="31" t="s">
         <v>193</v>
       </c>
-      <c r="P58" s="34" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q58" s="37">
+      <c r="P58" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q58" s="36">
         <v>25504</v>
       </c>
-      <c r="R58" s="32" t="s">
+      <c r="R58" s="31" t="s">
         <v>194</v>
       </c>
     </row>
@@ -4429,52 +4432,52 @@
       <c r="A59" s="19" t="s">
         <v>208</v>
       </c>
-      <c r="B59" s="33" t="s">
+      <c r="B59" s="32" t="s">
         <v>78</v>
       </c>
-      <c r="C59" s="32" t="s">
+      <c r="C59" s="31" t="s">
         <v>86</v>
       </c>
-      <c r="D59" s="34" t="s">
+      <c r="D59" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="E59" s="34" t="s">
+      <c r="E59" s="33" t="s">
         <v>75</v>
       </c>
-      <c r="F59" s="34" t="s">
-        <v>178</v>
-      </c>
-      <c r="G59" s="34" t="s">
-        <v>178</v>
-      </c>
-      <c r="H59" s="32">
+      <c r="F59" s="33" t="s">
+        <v>178</v>
+      </c>
+      <c r="G59" s="33" t="s">
+        <v>178</v>
+      </c>
+      <c r="H59" s="31">
         <v>-81.679554234298493</v>
       </c>
-      <c r="I59" s="32">
+      <c r="I59" s="31">
         <v>38.373735533484897</v>
       </c>
-      <c r="J59" s="21" t="s">
+      <c r="J59" t="s">
         <v>208</v>
       </c>
-      <c r="K59" s="32" t="s">
+      <c r="K59" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="L59" s="35">
+      <c r="L59" s="34">
         <v>14</v>
       </c>
-      <c r="M59" s="35">
+      <c r="M59" s="34">
         <v>49500</v>
       </c>
-      <c r="N59" s="42">
+      <c r="N59" s="40">
         <v>183279</v>
       </c>
-      <c r="O59" s="32" t="s">
+      <c r="O59" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="P59" s="34" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q59" s="37">
+      <c r="P59" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q59" s="36">
         <v>25387</v>
       </c>
     </row>
@@ -4482,52 +4485,52 @@
       <c r="A60" s="19" t="s">
         <v>216</v>
       </c>
-      <c r="B60" s="33" t="s">
+      <c r="B60" s="32" t="s">
         <v>78</v>
       </c>
-      <c r="C60" s="32" t="s">
+      <c r="C60" s="31" t="s">
         <v>199</v>
       </c>
-      <c r="D60" s="34" t="s">
+      <c r="D60" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="E60" s="34" t="s">
+      <c r="E60" s="33" t="s">
         <v>75</v>
       </c>
-      <c r="F60" s="34" t="s">
-        <v>178</v>
-      </c>
-      <c r="G60" s="34" t="s">
-        <v>178</v>
-      </c>
-      <c r="H60" s="32">
+      <c r="F60" s="33" t="s">
+        <v>178</v>
+      </c>
+      <c r="G60" s="33" t="s">
+        <v>178</v>
+      </c>
+      <c r="H60" s="31">
         <v>-81.758709180509001</v>
       </c>
-      <c r="I60" s="32">
+      <c r="I60" s="31">
         <v>38.368519014596998</v>
       </c>
-      <c r="J60" s="21" t="s">
+      <c r="J60" t="s">
         <v>216</v>
       </c>
-      <c r="K60" s="32" t="s">
+      <c r="K60" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="L60" s="35">
+      <c r="L60" s="34">
         <v>2.25</v>
       </c>
-      <c r="M60" s="35">
+      <c r="M60" s="34">
         <v>9000</v>
       </c>
-      <c r="N60" s="42">
+      <c r="N60" s="40">
         <v>183279</v>
       </c>
-      <c r="O60" s="36" t="s">
+      <c r="O60" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="P60" s="34" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q60" s="33">
+      <c r="P60" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q60" s="32">
         <v>25064</v>
       </c>
     </row>
@@ -4535,52 +4538,52 @@
       <c r="A61" s="19" t="s">
         <v>210</v>
       </c>
-      <c r="B61" s="33" t="s">
+      <c r="B61" s="32" t="s">
         <v>78</v>
       </c>
-      <c r="C61" s="32" t="s">
+      <c r="C61" s="31" t="s">
         <v>195</v>
       </c>
-      <c r="D61" s="34" t="s">
+      <c r="D61" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="E61" s="34" t="s">
+      <c r="E61" s="33" t="s">
         <v>75</v>
       </c>
-      <c r="F61" s="34" t="s">
-        <v>178</v>
-      </c>
-      <c r="G61" s="34" t="s">
-        <v>178</v>
-      </c>
-      <c r="H61" s="32">
+      <c r="F61" s="33" t="s">
+        <v>178</v>
+      </c>
+      <c r="G61" s="33" t="s">
+        <v>178</v>
+      </c>
+      <c r="H61" s="31">
         <v>-82.006959612418996</v>
       </c>
-      <c r="I61" s="32">
+      <c r="I61" s="31">
         <v>38.446524084559897</v>
       </c>
-      <c r="J61" s="21" t="s">
+      <c r="J61" t="s">
         <v>207</v>
       </c>
-      <c r="K61" s="32" t="s">
+      <c r="K61" s="31" t="s">
         <v>196</v>
       </c>
-      <c r="L61" s="35">
+      <c r="L61" s="34">
         <v>4.5</v>
       </c>
-      <c r="M61" s="35">
+      <c r="M61" s="34">
         <v>28759</v>
       </c>
-      <c r="N61" s="42">
+      <c r="N61" s="40">
         <v>55486</v>
       </c>
-      <c r="O61" s="36" t="s">
+      <c r="O61" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="P61" s="34" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q61" s="33">
+      <c r="P61" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q61" s="32">
         <v>25526</v>
       </c>
     </row>
@@ -4588,55 +4591,55 @@
       <c r="A62" s="19" t="s">
         <v>200</v>
       </c>
-      <c r="B62" s="33" t="s">
+      <c r="B62" s="32" t="s">
         <v>78</v>
       </c>
-      <c r="C62" s="32" t="s">
+      <c r="C62" s="31" t="s">
         <v>201</v>
       </c>
-      <c r="D62" s="34" t="s">
+      <c r="D62" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="E62" s="34" t="s">
+      <c r="E62" s="33" t="s">
         <v>76</v>
       </c>
-      <c r="F62" s="34" t="s">
-        <v>178</v>
-      </c>
-      <c r="G62" s="34" t="s">
-        <v>178</v>
-      </c>
-      <c r="H62" s="32">
+      <c r="F62" s="33" t="s">
+        <v>178</v>
+      </c>
+      <c r="G62" s="33" t="s">
+        <v>178</v>
+      </c>
+      <c r="H62" s="31">
         <v>-82.451303840583293</v>
       </c>
-      <c r="I62" s="32">
+      <c r="I62" s="31">
         <v>38.343336164586603</v>
       </c>
-      <c r="J62" s="21" t="s">
+      <c r="J62" t="s">
         <v>207</v>
       </c>
-      <c r="K62" s="32" t="s">
+      <c r="K62" s="31" t="s">
         <v>202</v>
       </c>
-      <c r="L62" s="41">
+      <c r="L62" s="39">
         <v>0.12</v>
       </c>
-      <c r="M62" s="41">
+      <c r="M62" s="39">
         <v>1600</v>
       </c>
-      <c r="N62" s="42">
+      <c r="N62" s="40">
         <v>42481</v>
       </c>
-      <c r="O62" s="36" t="s">
+      <c r="O62" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="P62" s="34" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q62" s="33">
+      <c r="P62" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q62" s="32">
         <v>25701</v>
       </c>
-      <c r="R62" s="32" t="s">
+      <c r="R62" s="31" t="s">
         <v>203</v>
       </c>
     </row>
@@ -4644,55 +4647,55 @@
       <c r="A63" s="19" t="s">
         <v>204</v>
       </c>
-      <c r="B63" s="33" t="s">
+      <c r="B63" s="32" t="s">
         <v>78</v>
       </c>
-      <c r="C63" s="32" t="s">
+      <c r="C63" s="31" t="s">
         <v>205</v>
       </c>
-      <c r="D63" s="34" t="s">
+      <c r="D63" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="E63" s="34" t="s">
+      <c r="E63" s="33" t="s">
         <v>75</v>
       </c>
-      <c r="F63" s="34" t="s">
-        <v>178</v>
-      </c>
-      <c r="G63" s="34" t="s">
-        <v>178</v>
-      </c>
-      <c r="H63" s="34">
+      <c r="F63" s="33" t="s">
+        <v>178</v>
+      </c>
+      <c r="G63" s="33" t="s">
+        <v>178</v>
+      </c>
+      <c r="H63" s="33">
         <v>-82.287563960345196</v>
       </c>
-      <c r="I63" s="32">
+      <c r="I63" s="31">
         <v>38.572623654172197</v>
       </c>
-      <c r="J63" s="21" t="s">
+      <c r="J63" t="s">
         <v>215</v>
       </c>
-      <c r="K63" s="32" t="s">
+      <c r="K63" s="31" t="s">
         <v>192</v>
       </c>
-      <c r="L63" s="35">
+      <c r="L63" s="34">
         <v>0.125</v>
       </c>
-      <c r="M63" s="35">
+      <c r="M63" s="34">
         <v>1000</v>
       </c>
-      <c r="N63" s="42">
+      <c r="N63" s="40">
         <v>96319</v>
       </c>
-      <c r="O63" s="36" t="s">
+      <c r="O63" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="P63" s="34" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q63" s="33">
+      <c r="P63" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q63" s="32">
         <v>25537</v>
       </c>
-      <c r="R63" s="32" t="s">
+      <c r="R63" s="31" t="s">
         <v>206</v>
       </c>
     </row>
@@ -4754,52 +4757,52 @@
       <c r="A65" s="19" t="s">
         <v>215</v>
       </c>
-      <c r="B65" s="33" t="s">
+      <c r="B65" s="32" t="s">
         <v>78</v>
       </c>
-      <c r="C65" s="32" t="s">
+      <c r="C65" s="31" t="s">
         <v>198</v>
       </c>
-      <c r="D65" s="34" t="s">
+      <c r="D65" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="E65" s="34" t="s">
+      <c r="E65" s="33" t="s">
         <v>75</v>
       </c>
-      <c r="F65" s="34" t="s">
-        <v>178</v>
-      </c>
-      <c r="G65" s="34" t="s">
-        <v>178</v>
-      </c>
-      <c r="H65" s="32">
+      <c r="F65" s="33" t="s">
+        <v>178</v>
+      </c>
+      <c r="G65" s="33" t="s">
+        <v>178</v>
+      </c>
+      <c r="H65" s="31">
         <v>-82.298209254857795</v>
       </c>
-      <c r="I65" s="32">
+      <c r="I65" s="31">
         <v>38.419661908139098</v>
       </c>
-      <c r="J65" s="21" t="s">
+      <c r="J65" t="s">
         <v>215</v>
       </c>
-      <c r="K65" s="32" t="s">
+      <c r="K65" s="31" t="s">
         <v>192</v>
       </c>
-      <c r="L65" s="35">
+      <c r="L65" s="34">
         <v>2.16</v>
       </c>
-      <c r="M65" s="35">
+      <c r="M65" s="34">
         <v>7000</v>
       </c>
-      <c r="N65" s="42">
+      <c r="N65" s="40">
         <v>96319</v>
       </c>
-      <c r="O65" s="36" t="s">
+      <c r="O65" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="P65" s="34" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q65" s="33">
+      <c r="P65" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q65" s="32">
         <v>25705</v>
       </c>
     </row>
@@ -4807,55 +4810,55 @@
       <c r="A66" s="19" t="s">
         <v>213</v>
       </c>
-      <c r="B66" s="33" t="s">
+      <c r="B66" s="32" t="s">
         <v>78</v>
       </c>
-      <c r="C66" s="32" t="s">
+      <c r="C66" s="31" t="s">
         <v>214</v>
       </c>
-      <c r="D66" s="34" t="s">
+      <c r="D66" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="E66" s="34" t="s">
+      <c r="E66" s="33" t="s">
         <v>75</v>
       </c>
-      <c r="F66" s="34" t="s">
-        <v>178</v>
-      </c>
-      <c r="G66" s="34" t="s">
-        <v>178</v>
-      </c>
-      <c r="H66" s="32">
+      <c r="F66" s="33" t="s">
+        <v>178</v>
+      </c>
+      <c r="G66" s="33" t="s">
+        <v>178</v>
+      </c>
+      <c r="H66" s="31">
         <v>-82.209446953848399</v>
       </c>
-      <c r="I66" s="32">
+      <c r="I66" s="31">
         <v>38.431960787764801</v>
       </c>
-      <c r="J66" s="21" t="s">
+      <c r="J66" t="s">
         <v>226</v>
       </c>
-      <c r="K66" s="32" t="s">
+      <c r="K66" s="31" t="s">
         <v>192</v>
       </c>
-      <c r="L66" s="35">
+      <c r="L66" s="34">
         <v>2.5</v>
       </c>
-      <c r="M66" s="35">
+      <c r="M66" s="34">
         <v>11250</v>
       </c>
-      <c r="N66" s="42">
+      <c r="N66" s="40">
         <v>96319</v>
       </c>
-      <c r="O66" s="36" t="s">
+      <c r="O66" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="P66" s="34" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q66" s="33">
+      <c r="P66" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q66" s="32">
         <v>25545</v>
       </c>
-      <c r="R66" s="32" t="s">
+      <c r="R66" s="31" t="s">
         <v>197</v>
       </c>
     </row>
@@ -4863,55 +4866,55 @@
       <c r="A67" s="19" t="s">
         <v>211</v>
       </c>
-      <c r="B67" s="33" t="s">
+      <c r="B67" s="32" t="s">
         <v>78</v>
       </c>
-      <c r="C67" s="32" t="s">
+      <c r="C67" s="31" t="s">
         <v>212</v>
       </c>
-      <c r="D67" s="34" t="s">
+      <c r="D67" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="E67" s="34" t="s">
+      <c r="E67" s="33" t="s">
         <v>75</v>
       </c>
-      <c r="F67" s="34" t="s">
-        <v>178</v>
-      </c>
-      <c r="G67" s="34" t="s">
-        <v>178</v>
-      </c>
-      <c r="H67" s="32">
+      <c r="F67" s="33" t="s">
+        <v>178</v>
+      </c>
+      <c r="G67" s="33" t="s">
+        <v>178</v>
+      </c>
+      <c r="H67" s="31">
         <v>-82.209446953848399</v>
       </c>
-      <c r="I67" s="32">
+      <c r="I67" s="31">
         <v>38.431960787764801</v>
       </c>
-      <c r="J67" s="21" t="s">
+      <c r="J67" t="s">
         <v>226</v>
       </c>
-      <c r="K67" s="32" t="s">
+      <c r="K67" s="31" t="s">
         <v>192</v>
       </c>
-      <c r="L67" s="35">
+      <c r="L67" s="34">
         <v>2.5</v>
       </c>
-      <c r="M67" s="35">
+      <c r="M67" s="34">
         <v>11250</v>
       </c>
-      <c r="N67" s="42">
+      <c r="N67" s="40">
         <v>96319</v>
       </c>
-      <c r="O67" s="36" t="s">
+      <c r="O67" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="P67" s="34" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q67" s="33">
+      <c r="P67" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q67" s="32">
         <v>25545</v>
       </c>
-      <c r="R67" s="32" t="s">
+      <c r="R67" s="31" t="s">
         <v>197</v>
       </c>
     </row>
@@ -4919,7 +4922,7 @@
       <c r="A68" s="20" t="s">
         <v>132</v>
       </c>
-      <c r="B68" s="22" t="s">
+      <c r="B68" s="21" t="s">
         <v>225</v>
       </c>
       <c r="C68" s="20" t="s">
@@ -4940,7 +4943,7 @@
       <c r="H68" s="20">
         <v>-79.936940000000007</v>
       </c>
-      <c r="I68" s="23">
+      <c r="I68" s="22">
         <v>39.022010000000002</v>
       </c>
       <c r="J68" s="20" t="s">
@@ -4949,20 +4952,20 @@
       <c r="K68" s="20" t="s">
         <v>143</v>
       </c>
-      <c r="L68" s="24">
+      <c r="L68" s="23">
         <v>0.36499999999999999</v>
       </c>
-      <c r="M68" s="25">
+      <c r="M68" s="24">
         <v>1974</v>
       </c>
-      <c r="N68" s="25">
+      <c r="N68" s="24">
         <v>16633</v>
       </c>
-      <c r="O68" s="39"/>
+      <c r="O68" s="20"/>
       <c r="P68" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="Q68" s="22">
+      <c r="Q68" s="21">
         <v>26250</v>
       </c>
       <c r="R68" s="20"/>
@@ -4971,7 +4974,7 @@
       <c r="A69" s="20" t="s">
         <v>130</v>
       </c>
-      <c r="B69" s="22" t="s">
+      <c r="B69" s="21" t="s">
         <v>225</v>
       </c>
       <c r="C69" s="20" t="s">
@@ -4992,7 +4995,7 @@
       <c r="H69" s="20">
         <v>-80.212010000000006</v>
       </c>
-      <c r="I69" s="23">
+      <c r="I69" s="22">
         <v>39.72007</v>
       </c>
       <c r="J69" s="20" t="s">
@@ -5001,20 +5004,20 @@
       <c r="K69" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="L69" s="24">
+      <c r="L69" s="23">
         <v>0.05</v>
       </c>
-      <c r="M69" s="24">
+      <c r="M69" s="23">
         <v>400</v>
       </c>
-      <c r="N69" s="25">
+      <c r="N69" s="24">
         <v>105612</v>
       </c>
       <c r="O69" s="20"/>
       <c r="P69" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="Q69" s="22">
+      <c r="Q69" s="21">
         <v>26521</v>
       </c>
       <c r="R69" s="20"/>
@@ -5023,7 +5026,7 @@
       <c r="A70" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="B70" s="22" t="s">
+      <c r="B70" s="21" t="s">
         <v>225</v>
       </c>
       <c r="C70" s="20" t="s">
@@ -5044,7 +5047,7 @@
       <c r="H70" s="20">
         <v>-80.258989999999997</v>
       </c>
-      <c r="I70" s="23">
+      <c r="I70" s="22">
         <v>39.280479999999997</v>
       </c>
       <c r="J70" s="20" t="s">
@@ -5053,13 +5056,13 @@
       <c r="K70" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="L70" s="24">
+      <c r="L70" s="23">
         <v>3</v>
       </c>
-      <c r="M70" s="25">
+      <c r="M70" s="24">
         <v>6984</v>
       </c>
-      <c r="N70" s="25">
+      <c r="N70" s="24">
         <v>67256</v>
       </c>
       <c r="O70" s="20" t="s">
@@ -5068,7 +5071,7 @@
       <c r="P70" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="Q70" s="22">
+      <c r="Q70" s="21">
         <v>26330</v>
       </c>
       <c r="R70" s="20"/>
@@ -5077,7 +5080,7 @@
       <c r="A71" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="B71" s="22" t="s">
+      <c r="B71" s="21" t="s">
         <v>225</v>
       </c>
       <c r="C71" s="20" t="s">
@@ -5098,7 +5101,7 @@
       <c r="H71" s="20">
         <v>-80.567440000000005</v>
       </c>
-      <c r="I71" s="23">
+      <c r="I71" s="22">
         <v>39.826610000000002</v>
       </c>
       <c r="J71" s="20" t="s">
@@ -5107,22 +5110,22 @@
       <c r="K71" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="L71" s="24">
+      <c r="L71" s="23">
         <v>0.21</v>
       </c>
-      <c r="M71" s="25">
+      <c r="M71" s="24">
         <v>1340</v>
       </c>
-      <c r="N71" s="25">
+      <c r="N71" s="24">
         <v>30531</v>
       </c>
-      <c r="O71" s="40" t="s">
+      <c r="O71" s="38" t="s">
         <v>18</v>
       </c>
       <c r="P71" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="Q71" s="22">
+      <c r="Q71" s="21">
         <v>26033</v>
       </c>
       <c r="R71" s="20"/>
@@ -5131,7 +5134,7 @@
       <c r="A72" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="B72" s="22" t="s">
+      <c r="B72" s="21" t="s">
         <v>225</v>
       </c>
       <c r="C72" s="20" t="s">
@@ -5152,7 +5155,7 @@
       <c r="H72" s="20">
         <v>-80.124449999999996</v>
       </c>
-      <c r="I72" s="23">
+      <c r="I72" s="22">
         <v>39.493949999999998</v>
       </c>
       <c r="J72" s="20" t="s">
@@ -5161,22 +5164,22 @@
       <c r="K72" s="20" t="s">
         <v>107</v>
       </c>
-      <c r="L72" s="24">
+      <c r="L72" s="23">
         <v>9</v>
       </c>
-      <c r="M72" s="25">
+      <c r="M72" s="24">
         <v>25525</v>
       </c>
-      <c r="N72" s="25">
+      <c r="N72" s="24">
         <v>56072</v>
       </c>
-      <c r="O72" s="40" t="s">
+      <c r="O72" s="38" t="s">
         <v>18</v>
       </c>
       <c r="P72" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="Q72" s="22">
+      <c r="Q72" s="21">
         <v>26554</v>
       </c>
       <c r="R72" s="20"/>
@@ -5185,7 +5188,7 @@
       <c r="A73" s="20" t="s">
         <v>146</v>
       </c>
-      <c r="B73" s="22" t="s">
+      <c r="B73" s="21" t="s">
         <v>225</v>
       </c>
       <c r="C73" s="20" t="s">
@@ -5211,24 +5214,26 @@
       <c r="K73" s="20" t="s">
         <v>151</v>
       </c>
-      <c r="L73" s="24">
+      <c r="L73" s="23">
         <v>0.3</v>
       </c>
-      <c r="M73" s="25">
+      <c r="M73" s="24">
         <v>1800</v>
       </c>
-      <c r="N73" s="25">
+      <c r="N73" s="24">
         <v>8811</v>
       </c>
       <c r="O73" s="20"/>
-      <c r="P73" s="20"/>
-      <c r="Q73" s="22"/>
+      <c r="P73" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q73" s="21"/>
     </row>
     <row r="74" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A74" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="B74" s="22" t="s">
+      <c r="B74" s="21" t="s">
         <v>225</v>
       </c>
       <c r="C74" s="20" t="s">
@@ -5249,7 +5254,7 @@
       <c r="H74" s="20">
         <v>-80.260360000000006</v>
       </c>
-      <c r="I74" s="23">
+      <c r="I74" s="22">
         <v>39.452579999999998</v>
       </c>
       <c r="J74" s="20" t="s">
@@ -5258,22 +5263,22 @@
       <c r="K74" s="20" t="s">
         <v>107</v>
       </c>
-      <c r="L74" s="24">
+      <c r="L74" s="23">
         <v>0.1</v>
       </c>
-      <c r="M74" s="25">
+      <c r="M74" s="24">
         <v>2742</v>
       </c>
-      <c r="N74" s="25">
+      <c r="N74" s="24">
         <v>56072</v>
       </c>
-      <c r="O74" s="40" t="s">
+      <c r="O74" s="38" t="s">
         <v>18</v>
       </c>
       <c r="P74" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="Q74" s="22">
+      <c r="Q74" s="21">
         <v>26591</v>
       </c>
       <c r="R74" s="20"/>

</xml_diff>

<commit_message>
Integration of MU data, with some bugs to squash still.
</commit_message>
<xml_diff>
--- a/analysis/resources/WaTCH_Tables.xlsx
+++ b/analysis/resources/WaTCH_Tables.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tpd0001/github/watch-wv/analysis/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49956801-D481-F444-96D6-4EB217BE7678}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCBF2398-40A2-E541-A404-164EB4BB78D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="600" yWindow="760" windowWidth="26960" windowHeight="18880" xr2:uid="{ABEE2980-A2EF-284E-9534-8BF6C1D1D8CC}"/>
   </bookViews>
@@ -1026,7 +1026,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1314,7 +1314,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1325,10 +1325,10 @@
   <dimension ref="A1:R74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="M19" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B55" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Q49" sqref="Q49"/>
+      <selection pane="bottomRight" activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3416,7 +3416,7 @@
         <v>207</v>
       </c>
       <c r="B40" s="32" t="s">
-        <v>78</v>
+        <v>122</v>
       </c>
       <c r="C40" s="31" t="s">
         <v>190</v>
@@ -4376,8 +4376,8 @@
       <c r="A58" s="19" t="s">
         <v>209</v>
       </c>
-      <c r="B58" s="32" t="s">
-        <v>78</v>
+      <c r="B58" s="3" t="s">
+        <v>122</v>
       </c>
       <c r="C58" s="31" t="s">
         <v>191</v>
@@ -4432,8 +4432,8 @@
       <c r="A59" s="19" t="s">
         <v>208</v>
       </c>
-      <c r="B59" s="32" t="s">
-        <v>78</v>
+      <c r="B59" s="3" t="s">
+        <v>122</v>
       </c>
       <c r="C59" s="31" t="s">
         <v>86</v>
@@ -4485,8 +4485,8 @@
       <c r="A60" s="19" t="s">
         <v>216</v>
       </c>
-      <c r="B60" s="32" t="s">
-        <v>78</v>
+      <c r="B60" s="3" t="s">
+        <v>122</v>
       </c>
       <c r="C60" s="31" t="s">
         <v>199</v>
@@ -4538,8 +4538,8 @@
       <c r="A61" s="19" t="s">
         <v>210</v>
       </c>
-      <c r="B61" s="32" t="s">
-        <v>78</v>
+      <c r="B61" s="3" t="s">
+        <v>122</v>
       </c>
       <c r="C61" s="31" t="s">
         <v>195</v>
@@ -4591,8 +4591,8 @@
       <c r="A62" s="19" t="s">
         <v>200</v>
       </c>
-      <c r="B62" s="32" t="s">
-        <v>78</v>
+      <c r="B62" s="3" t="s">
+        <v>122</v>
       </c>
       <c r="C62" s="31" t="s">
         <v>201</v>
@@ -4647,8 +4647,8 @@
       <c r="A63" s="19" t="s">
         <v>204</v>
       </c>
-      <c r="B63" s="32" t="s">
-        <v>78</v>
+      <c r="B63" s="3" t="s">
+        <v>122</v>
       </c>
       <c r="C63" s="31" t="s">
         <v>205</v>
@@ -4703,7 +4703,7 @@
       <c r="A64" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="B64" s="6" t="s">
+      <c r="B64" s="3" t="s">
         <v>78</v>
       </c>
       <c r="C64" s="4" t="s">
@@ -4757,8 +4757,8 @@
       <c r="A65" s="19" t="s">
         <v>215</v>
       </c>
-      <c r="B65" s="32" t="s">
-        <v>78</v>
+      <c r="B65" s="3" t="s">
+        <v>122</v>
       </c>
       <c r="C65" s="31" t="s">
         <v>198</v>
@@ -4810,8 +4810,8 @@
       <c r="A66" s="19" t="s">
         <v>213</v>
       </c>
-      <c r="B66" s="32" t="s">
-        <v>78</v>
+      <c r="B66" s="3" t="s">
+        <v>122</v>
       </c>
       <c r="C66" s="31" t="s">
         <v>214</v>
@@ -4866,8 +4866,8 @@
       <c r="A67" s="19" t="s">
         <v>211</v>
       </c>
-      <c r="B67" s="32" t="s">
-        <v>78</v>
+      <c r="B67" s="3" t="s">
+        <v>122</v>
       </c>
       <c r="C67" s="31" t="s">
         <v>212</v>

</xml_diff>

<commit_message>
Data update 3/30/23 run.
</commit_message>
<xml_diff>
--- a/analysis/resources/WaTCH_Tables.xlsx
+++ b/analysis/resources/WaTCH_Tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tpd0001/github/watch-wv/analysis/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCBF2398-40A2-E541-A404-164EB4BB78D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D90E945-1958-E14E-88D6-DB1F1691B4B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="760" windowWidth="26960" windowHeight="18880" xr2:uid="{ABEE2980-A2EF-284E-9534-8BF6C1D1D8CC}"/>
+    <workbookView xWindow="580" yWindow="760" windowWidth="26960" windowHeight="18880" xr2:uid="{ABEE2980-A2EF-284E-9534-8BF6C1D1D8CC}"/>
   </bookViews>
   <sheets>
     <sheet name="locations" sheetId="1" r:id="rId1"/>
@@ -1325,10 +1325,10 @@
   <dimension ref="A1:R74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B55" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B41" sqref="B41"/>
+      <selection pane="bottomRight" activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2876,7 +2876,7 @@
         <v>23</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>122</v>
+        <v>78</v>
       </c>
       <c r="C30" t="s">
         <v>83</v>
@@ -3309,7 +3309,7 @@
         <v>131</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>122</v>
+        <v>78</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>138</v>
@@ -4065,7 +4065,7 @@
         <v>66</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>122</v>
+        <v>78</v>
       </c>
       <c r="C52" s="4" t="s">
         <v>97</v>
@@ -4118,7 +4118,7 @@
         <v>12</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>122</v>
+        <v>78</v>
       </c>
       <c r="C53" s="4" t="s">
         <v>101</v>

</xml_diff>

<commit_message>
Data update for 8/26.
</commit_message>
<xml_diff>
--- a/analysis/resources/WaTCH_Tables.xlsx
+++ b/analysis/resources/WaTCH_Tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tpd0001/github/watch-wv/analysis/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F2EF8A6-1307-1944-8721-A199F522FDBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0308033-4670-2944-9017-E626F6BBC93E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{ABEE2980-A2EF-284E-9534-8BF6C1D1D8CC}"/>
   </bookViews>
@@ -1562,10 +1562,10 @@
   <dimension ref="A1:U75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B25" sqref="B25"/>
+      <selection pane="bottomRight" activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Data update through 20-Sep-2023.
</commit_message>
<xml_diff>
--- a/analysis/resources/WaTCH_Tables.xlsx
+++ b/analysis/resources/WaTCH_Tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tpd0001/github/watch-wv/analysis/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0308033-4670-2944-9017-E626F6BBC93E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D189EE53-A178-3847-AA2D-A27EF02D916B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{ABEE2980-A2EF-284E-9534-8BF6C1D1D8CC}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30040" windowHeight="14260" xr2:uid="{ABEE2980-A2EF-284E-9534-8BF6C1D1D8CC}"/>
   </bookViews>
   <sheets>
     <sheet name="locations" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="898" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="911" uniqueCount="302">
   <si>
     <t>capacity_mgd</t>
   </si>
@@ -925,6 +925,21 @@
   </si>
   <si>
     <t>54079-002-01-00-00</t>
+  </si>
+  <si>
+    <t>WhiteOakWWTP-01</t>
+  </si>
+  <si>
+    <t>White Oak</t>
+  </si>
+  <si>
+    <t>Fayette</t>
+  </si>
+  <si>
+    <t>WV0044041</t>
+  </si>
+  <si>
+    <t>54019-001-01-00-00</t>
   </si>
 </sst>
 </file>
@@ -1559,13 +1574,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0856F7A-D0C0-3942-9027-9FB2F3C2C3E0}">
-  <dimension ref="A1:U75"/>
+  <dimension ref="A1:U76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B16" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D30" sqref="D30"/>
+      <selection pane="bottomRight" activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3517,116 +3532,122 @@
       </c>
       <c r="U31"/>
     </row>
-    <row r="32" spans="1:21" s="25" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="42" t="s">
+    <row r="32" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="18" t="s">
+        <v>297</v>
+      </c>
+      <c r="B32" t="s">
+        <v>301</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="E32" s="32" t="s">
+        <v>300</v>
+      </c>
+      <c r="F32" s="32">
+        <v>54001022001</v>
+      </c>
+      <c r="G32" t="s">
+        <v>26</v>
+      </c>
+      <c r="H32" t="s">
+        <v>75</v>
+      </c>
+      <c r="I32" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="J32" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="K32">
+        <v>-81.1824412</v>
+      </c>
+      <c r="L32">
+        <v>37.946477700000003</v>
+      </c>
+      <c r="M32" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="N32" t="s">
+        <v>299</v>
+      </c>
+      <c r="O32" s="17">
+        <v>0.75</v>
+      </c>
+      <c r="P32" s="14">
+        <v>2626</v>
+      </c>
+      <c r="Q32" s="14">
+        <v>40488</v>
+      </c>
+      <c r="R32" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="S32" t="s">
+        <v>31</v>
+      </c>
+      <c r="T32" s="3">
+        <v>25917</v>
+      </c>
+      <c r="U32"/>
+    </row>
+    <row r="33" spans="1:21" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="42" t="s">
         <v>216</v>
       </c>
-      <c r="B32" s="42"/>
-      <c r="C32" s="43" t="s">
+      <c r="B33" s="42"/>
+      <c r="C33" s="43" t="s">
         <v>78</v>
       </c>
-      <c r="D32" s="42" t="s">
+      <c r="D33" s="42" t="s">
         <v>217</v>
       </c>
-      <c r="E32" s="42"/>
-      <c r="F32" s="42"/>
-      <c r="G32" s="42" t="s">
+      <c r="E33" s="42"/>
+      <c r="F33" s="42"/>
+      <c r="G33" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="H32" s="42" t="s">
+      <c r="H33" s="42" t="s">
         <v>76</v>
       </c>
-      <c r="I32" s="42" t="s">
+      <c r="I33" s="42" t="s">
         <v>185</v>
       </c>
-      <c r="J32" s="42" t="s">
+      <c r="J33" s="42" t="s">
         <v>179</v>
       </c>
-      <c r="K32" s="42"/>
-      <c r="L32" s="42"/>
-      <c r="M32" s="42"/>
-      <c r="N32" s="42" t="s">
+      <c r="K33" s="42"/>
+      <c r="L33" s="42"/>
+      <c r="M33" s="42"/>
+      <c r="N33" s="42" t="s">
         <v>191</v>
       </c>
-      <c r="O32" s="44"/>
-      <c r="P32" s="44"/>
-      <c r="Q32" s="50">
+      <c r="O33" s="44"/>
+      <c r="P33" s="44"/>
+      <c r="Q33" s="50">
         <v>96319</v>
       </c>
-      <c r="R32" s="42"/>
-      <c r="S32" s="42" t="s">
-        <v>31</v>
-      </c>
-      <c r="T32" s="43"/>
-      <c r="U32" s="42"/>
-    </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A33" s="39" t="s">
-        <v>49</v>
-      </c>
-      <c r="B33" s="39"/>
-      <c r="C33" s="47" t="s">
-        <v>78</v>
-      </c>
-      <c r="D33" s="39" t="s">
-        <v>84</v>
-      </c>
-      <c r="E33" s="39"/>
-      <c r="F33" s="39"/>
-      <c r="G33" s="39" t="s">
-        <v>48</v>
-      </c>
-      <c r="H33" s="39" t="s">
-        <v>76</v>
-      </c>
-      <c r="I33" s="39" t="s">
-        <v>185</v>
-      </c>
-      <c r="J33" s="39" t="s">
-        <v>180</v>
-      </c>
-      <c r="K33" s="39">
-        <v>-79.905010000000004</v>
-      </c>
-      <c r="L33" s="39">
-        <v>39.610210000000002</v>
-      </c>
-      <c r="M33" s="39" t="s">
-        <v>14</v>
-      </c>
-      <c r="N33" s="39" t="s">
-        <v>15</v>
-      </c>
-      <c r="O33" s="48">
-        <v>-1</v>
-      </c>
-      <c r="P33" s="48">
-        <v>579</v>
-      </c>
-      <c r="Q33" s="49">
-        <v>105612</v>
-      </c>
-      <c r="R33" s="39" t="s">
-        <v>55</v>
-      </c>
-      <c r="S33" s="39" t="s">
-        <v>31</v>
-      </c>
-      <c r="T33" s="47">
-        <v>26508</v>
-      </c>
-      <c r="U33" s="39"/>
+      <c r="R33" s="42"/>
+      <c r="S33" s="42" t="s">
+        <v>31</v>
+      </c>
+      <c r="T33" s="43"/>
+      <c r="U33" s="42"/>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A34" s="39" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B34" s="39"/>
       <c r="C34" s="47" t="s">
         <v>78</v>
       </c>
       <c r="D34" s="39" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E34" s="39"/>
       <c r="F34" s="39"/>
@@ -3643,10 +3664,10 @@
         <v>180</v>
       </c>
       <c r="K34" s="39">
-        <v>-79.867609999999999</v>
+        <v>-79.905010000000004</v>
       </c>
       <c r="L34" s="39">
-        <v>39.652670000000001</v>
+        <v>39.610210000000002</v>
       </c>
       <c r="M34" s="39" t="s">
         <v>14</v>
@@ -3658,7 +3679,7 @@
         <v>-1</v>
       </c>
       <c r="P34" s="48">
-        <v>830</v>
+        <v>579</v>
       </c>
       <c r="Q34" s="49">
         <v>105612</v>
@@ -3674,75 +3695,73 @@
       </c>
       <c r="U34" s="39"/>
     </row>
-    <row r="35" spans="1:21" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="42" t="s">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A35" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="B35" s="39"/>
+      <c r="C35" s="47" t="s">
+        <v>78</v>
+      </c>
+      <c r="D35" s="39" t="s">
+        <v>88</v>
+      </c>
+      <c r="E35" s="39"/>
+      <c r="F35" s="39"/>
+      <c r="G35" s="39" t="s">
+        <v>48</v>
+      </c>
+      <c r="H35" s="39" t="s">
+        <v>76</v>
+      </c>
+      <c r="I35" s="39" t="s">
+        <v>185</v>
+      </c>
+      <c r="J35" s="39" t="s">
+        <v>180</v>
+      </c>
+      <c r="K35" s="39">
+        <v>-79.867609999999999</v>
+      </c>
+      <c r="L35" s="39">
+        <v>39.652670000000001</v>
+      </c>
+      <c r="M35" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="N35" s="39" t="s">
+        <v>15</v>
+      </c>
+      <c r="O35" s="48">
+        <v>-1</v>
+      </c>
+      <c r="P35" s="48">
+        <v>830</v>
+      </c>
+      <c r="Q35" s="49">
+        <v>105612</v>
+      </c>
+      <c r="R35" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="S35" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="T35" s="47">
+        <v>26508</v>
+      </c>
+      <c r="U35" s="39"/>
+    </row>
+    <row r="36" spans="1:21" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="42" t="s">
         <v>32</v>
-      </c>
-      <c r="B35" s="42"/>
-      <c r="C35" s="43" t="s">
-        <v>78</v>
-      </c>
-      <c r="D35" s="42" t="s">
-        <v>234</v>
-      </c>
-      <c r="E35" s="42"/>
-      <c r="F35" s="42"/>
-      <c r="G35" s="42" t="s">
-        <v>27</v>
-      </c>
-      <c r="H35" s="42" t="s">
-        <v>76</v>
-      </c>
-      <c r="I35" s="42" t="s">
-        <v>185</v>
-      </c>
-      <c r="J35" s="42" t="s">
-        <v>179</v>
-      </c>
-      <c r="K35" s="42">
-        <v>-79.945801900000006</v>
-      </c>
-      <c r="L35" s="42">
-        <v>39.6362083</v>
-      </c>
-      <c r="M35" s="42" t="s">
-        <v>14</v>
-      </c>
-      <c r="N35" s="42" t="s">
-        <v>15</v>
-      </c>
-      <c r="O35" s="44">
-        <v>-1</v>
-      </c>
-      <c r="P35" s="44">
-        <v>567</v>
-      </c>
-      <c r="Q35" s="45">
-        <v>105612</v>
-      </c>
-      <c r="R35" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="S35" s="42" t="s">
-        <v>31</v>
-      </c>
-      <c r="T35" s="43">
-        <v>26505</v>
-      </c>
-      <c r="U35" s="42" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A36" s="42" t="s">
-        <v>222</v>
       </c>
       <c r="B36" s="42"/>
       <c r="C36" s="43" t="s">
         <v>78</v>
       </c>
       <c r="D36" s="42" t="s">
-        <v>223</v>
+        <v>234</v>
       </c>
       <c r="E36" s="42"/>
       <c r="F36" s="42"/>
@@ -3758,34 +3777,50 @@
       <c r="J36" s="42" t="s">
         <v>179</v>
       </c>
-      <c r="K36" s="42"/>
-      <c r="L36" s="42"/>
-      <c r="M36" s="42"/>
+      <c r="K36" s="42">
+        <v>-79.945801900000006</v>
+      </c>
+      <c r="L36" s="42">
+        <v>39.6362083</v>
+      </c>
+      <c r="M36" s="42" t="s">
+        <v>14</v>
+      </c>
       <c r="N36" s="42" t="s">
-        <v>191</v>
-      </c>
-      <c r="O36" s="44"/>
-      <c r="P36" s="44"/>
-      <c r="Q36" s="50">
-        <v>96319</v>
-      </c>
-      <c r="R36" s="42"/>
+        <v>15</v>
+      </c>
+      <c r="O36" s="44">
+        <v>-1</v>
+      </c>
+      <c r="P36" s="44">
+        <v>567</v>
+      </c>
+      <c r="Q36" s="45">
+        <v>105612</v>
+      </c>
+      <c r="R36" s="42" t="s">
+        <v>47</v>
+      </c>
       <c r="S36" s="42" t="s">
         <v>31</v>
       </c>
-      <c r="T36" s="43"/>
-      <c r="U36" s="42"/>
+      <c r="T36" s="43">
+        <v>26505</v>
+      </c>
+      <c r="U36" s="42" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A37" s="42" t="s">
-        <v>38</v>
+        <v>222</v>
       </c>
       <c r="B37" s="42"/>
       <c r="C37" s="43" t="s">
         <v>78</v>
       </c>
       <c r="D37" s="42" t="s">
-        <v>166</v>
+        <v>223</v>
       </c>
       <c r="E37" s="42"/>
       <c r="F37" s="42"/>
@@ -3801,50 +3836,34 @@
       <c r="J37" s="42" t="s">
         <v>179</v>
       </c>
-      <c r="K37" s="42">
-        <v>-79.953093199999998</v>
-      </c>
-      <c r="L37" s="42">
-        <v>39.636423100000002</v>
-      </c>
-      <c r="M37" s="42" t="s">
-        <v>14</v>
-      </c>
+      <c r="K37" s="42"/>
+      <c r="L37" s="42"/>
+      <c r="M37" s="42"/>
       <c r="N37" s="42" t="s">
-        <v>15</v>
-      </c>
-      <c r="O37" s="44">
-        <v>-1</v>
-      </c>
-      <c r="P37" s="44">
-        <v>639</v>
-      </c>
-      <c r="Q37" s="45">
-        <v>105612</v>
-      </c>
-      <c r="R37" s="42" t="s">
-        <v>47</v>
-      </c>
+        <v>191</v>
+      </c>
+      <c r="O37" s="44"/>
+      <c r="P37" s="44"/>
+      <c r="Q37" s="50">
+        <v>96319</v>
+      </c>
+      <c r="R37" s="42"/>
       <c r="S37" s="42" t="s">
         <v>31</v>
       </c>
-      <c r="T37" s="43">
-        <v>26505</v>
-      </c>
-      <c r="U37" s="42" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="38" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="T37" s="43"/>
+      <c r="U37" s="42"/>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A38" s="42" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B38" s="42"/>
       <c r="C38" s="43" t="s">
         <v>78</v>
       </c>
       <c r="D38" s="42" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E38" s="42"/>
       <c r="F38" s="42"/>
@@ -3861,10 +3880,10 @@
         <v>179</v>
       </c>
       <c r="K38" s="42">
-        <v>-80.000420899999995</v>
+        <v>-79.953093199999998</v>
       </c>
       <c r="L38" s="42">
-        <v>39.6535571</v>
+        <v>39.636423100000002</v>
       </c>
       <c r="M38" s="42" t="s">
         <v>14</v>
@@ -3876,7 +3895,7 @@
         <v>-1</v>
       </c>
       <c r="P38" s="44">
-        <v>912</v>
+        <v>639</v>
       </c>
       <c r="Q38" s="45">
         <v>105612</v>
@@ -3891,137 +3910,137 @@
         <v>26505</v>
       </c>
       <c r="U38" s="42" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="42" t="s">
+        <v>39</v>
+      </c>
+      <c r="B39" s="42"/>
+      <c r="C39" s="43" t="s">
+        <v>78</v>
+      </c>
+      <c r="D39" s="42" t="s">
+        <v>167</v>
+      </c>
+      <c r="E39" s="42"/>
+      <c r="F39" s="42"/>
+      <c r="G39" s="42" t="s">
+        <v>27</v>
+      </c>
+      <c r="H39" s="42" t="s">
+        <v>76</v>
+      </c>
+      <c r="I39" s="42" t="s">
+        <v>185</v>
+      </c>
+      <c r="J39" s="42" t="s">
+        <v>179</v>
+      </c>
+      <c r="K39" s="42">
+        <v>-80.000420899999995</v>
+      </c>
+      <c r="L39" s="42">
+        <v>39.6535571</v>
+      </c>
+      <c r="M39" s="42" t="s">
+        <v>14</v>
+      </c>
+      <c r="N39" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="O39" s="44">
+        <v>-1</v>
+      </c>
+      <c r="P39" s="44">
+        <v>912</v>
+      </c>
+      <c r="Q39" s="45">
+        <v>105612</v>
+      </c>
+      <c r="R39" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="S39" s="42" t="s">
+        <v>31</v>
+      </c>
+      <c r="T39" s="43">
+        <v>26505</v>
+      </c>
+      <c r="U39" s="42" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A39" s="39" t="s">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A40" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="B39" s="39"/>
-      <c r="C39" s="47" t="s">
+      <c r="B40" s="39"/>
+      <c r="C40" s="47" t="s">
         <v>78</v>
       </c>
-      <c r="D39" s="39" t="s">
+      <c r="D40" s="39" t="s">
         <v>162</v>
       </c>
-      <c r="E39" s="39"/>
-      <c r="F39" s="39"/>
-      <c r="G39" s="39" t="s">
+      <c r="E40" s="39"/>
+      <c r="F40" s="39"/>
+      <c r="G40" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="H39" s="39" t="s">
+      <c r="H40" s="39" t="s">
         <v>76</v>
       </c>
-      <c r="I39" s="39" t="s">
+      <c r="I40" s="39" t="s">
         <v>185</v>
       </c>
-      <c r="J39" s="39" t="s">
+      <c r="J40" s="39" t="s">
         <v>184</v>
       </c>
-      <c r="K39" s="39">
+      <c r="K40" s="39">
         <v>-79.972157499999994</v>
       </c>
-      <c r="L39" s="39">
+      <c r="L40" s="39">
         <v>39.650096900000001</v>
       </c>
-      <c r="M39" s="39" t="s">
+      <c r="M40" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="N39" s="39" t="s">
+      <c r="N40" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="O39" s="48">
+      <c r="O40" s="48">
         <v>-1</v>
       </c>
-      <c r="P39" s="48">
+      <c r="P40" s="48">
         <v>-1</v>
       </c>
-      <c r="Q39" s="49">
+      <c r="Q40" s="49">
         <v>105612</v>
       </c>
-      <c r="R39" s="39" t="s">
+      <c r="R40" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="S39" s="39" t="s">
-        <v>31</v>
-      </c>
-      <c r="T39" s="47">
+      <c r="S40" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="T40" s="47">
         <v>26505</v>
       </c>
-      <c r="U39" s="39" t="s">
+      <c r="U40" s="39" t="s">
         <v>154</v>
-      </c>
-    </row>
-    <row r="40" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="42" t="s">
-        <v>40</v>
-      </c>
-      <c r="B40" s="42"/>
-      <c r="C40" s="43" t="s">
-        <v>78</v>
-      </c>
-      <c r="D40" s="42" t="s">
-        <v>169</v>
-      </c>
-      <c r="E40" s="42"/>
-      <c r="F40" s="42"/>
-      <c r="G40" s="42" t="s">
-        <v>27</v>
-      </c>
-      <c r="H40" s="42" t="s">
-        <v>76</v>
-      </c>
-      <c r="I40" s="42" t="s">
-        <v>185</v>
-      </c>
-      <c r="J40" s="42" t="s">
-        <v>179</v>
-      </c>
-      <c r="K40" s="42">
-        <v>-79.956234100000003</v>
-      </c>
-      <c r="L40" s="42">
-        <v>39.667909799999997</v>
-      </c>
-      <c r="M40" s="42" t="s">
-        <v>14</v>
-      </c>
-      <c r="N40" s="42" t="s">
-        <v>15</v>
-      </c>
-      <c r="O40" s="44">
-        <v>-1</v>
-      </c>
-      <c r="P40" s="44">
-        <v>-1</v>
-      </c>
-      <c r="Q40" s="45">
-        <v>105612</v>
-      </c>
-      <c r="R40" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="S40" s="42" t="s">
-        <v>31</v>
-      </c>
-      <c r="T40" s="43">
-        <v>26505</v>
-      </c>
-      <c r="U40" s="42" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="41" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="42" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B41" s="42"/>
       <c r="C41" s="43" t="s">
         <v>78</v>
       </c>
       <c r="D41" s="42" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E41" s="42"/>
       <c r="F41" s="42"/>
@@ -4038,10 +4057,10 @@
         <v>179</v>
       </c>
       <c r="K41" s="42">
-        <v>-79.956204600000007</v>
+        <v>-79.956234100000003</v>
       </c>
       <c r="L41" s="42">
-        <v>39.668112200000003</v>
+        <v>39.667909799999997</v>
       </c>
       <c r="M41" s="42" t="s">
         <v>14</v>
@@ -4068,24 +4087,24 @@
         <v>26505</v>
       </c>
       <c r="U41" s="42" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="42" spans="1:21" s="42" customFormat="1" x14ac:dyDescent="0.2">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="42" t="s">
-        <v>125</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="B42" s="42"/>
       <c r="C42" s="43" t="s">
         <v>78</v>
       </c>
       <c r="D42" s="42" t="s">
-        <v>134</v>
-      </c>
-      <c r="F42" s="42">
-        <v>54003906001</v>
-      </c>
+        <v>168</v>
+      </c>
+      <c r="E42" s="42"/>
+      <c r="F42" s="42"/>
       <c r="G42" s="42" t="s">
-        <v>144</v>
+        <v>27</v>
       </c>
       <c r="H42" s="42" t="s">
         <v>76</v>
@@ -4094,105 +4113,105 @@
         <v>185</v>
       </c>
       <c r="J42" s="42" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="K42" s="42">
-        <v>-79.515240000000006</v>
-      </c>
-      <c r="L42" s="51">
-        <v>39.66807</v>
+        <v>-79.956204600000007</v>
+      </c>
+      <c r="L42" s="42">
+        <v>39.668112200000003</v>
       </c>
       <c r="M42" s="42" t="s">
-        <v>145</v>
+        <v>14</v>
       </c>
       <c r="N42" s="42" t="s">
-        <v>81</v>
+        <v>15</v>
       </c>
       <c r="O42" s="44">
         <v>-1</v>
       </c>
-      <c r="P42" s="45">
+      <c r="P42" s="44">
+        <v>-1</v>
+      </c>
+      <c r="Q42" s="45">
+        <v>105612</v>
+      </c>
+      <c r="R42" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="S42" s="42" t="s">
+        <v>31</v>
+      </c>
+      <c r="T42" s="43">
+        <v>26505</v>
+      </c>
+      <c r="U42" s="42" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21" s="42" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="42" t="s">
+        <v>125</v>
+      </c>
+      <c r="C43" s="43" t="s">
+        <v>78</v>
+      </c>
+      <c r="D43" s="42" t="s">
+        <v>134</v>
+      </c>
+      <c r="F43" s="42">
+        <v>54003906001</v>
+      </c>
+      <c r="G43" s="42" t="s">
+        <v>144</v>
+      </c>
+      <c r="H43" s="42" t="s">
+        <v>76</v>
+      </c>
+      <c r="I43" s="42" t="s">
+        <v>185</v>
+      </c>
+      <c r="J43" s="42" t="s">
+        <v>183</v>
+      </c>
+      <c r="K43" s="42">
+        <v>-79.515240000000006</v>
+      </c>
+      <c r="L43" s="51">
+        <v>39.66807</v>
+      </c>
+      <c r="M43" s="42" t="s">
+        <v>145</v>
+      </c>
+      <c r="N43" s="42" t="s">
+        <v>81</v>
+      </c>
+      <c r="O43" s="44">
+        <v>-1</v>
+      </c>
+      <c r="P43" s="45">
         <v>1948</v>
       </c>
-      <c r="Q42" s="45">
+      <c r="Q43" s="45">
         <v>33432</v>
       </c>
-      <c r="S42" s="42" t="s">
-        <v>31</v>
-      </c>
-      <c r="T42" s="43">
+      <c r="S43" s="42" t="s">
+        <v>31</v>
+      </c>
+      <c r="T43" s="43">
         <v>26525</v>
-      </c>
-    </row>
-    <row r="43" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="39" t="s">
-        <v>34</v>
-      </c>
-      <c r="B43" s="39"/>
-      <c r="C43" s="47" t="s">
-        <v>78</v>
-      </c>
-      <c r="D43" s="39" t="s">
-        <v>163</v>
-      </c>
-      <c r="E43" s="39"/>
-      <c r="F43" s="39"/>
-      <c r="G43" s="39" t="s">
-        <v>27</v>
-      </c>
-      <c r="H43" s="39" t="s">
-        <v>76</v>
-      </c>
-      <c r="I43" s="39" t="s">
-        <v>185</v>
-      </c>
-      <c r="J43" s="39" t="s">
-        <v>179</v>
-      </c>
-      <c r="K43" s="39">
-        <v>-79.956762600000005</v>
-      </c>
-      <c r="L43" s="39">
-        <v>39.637875299999997</v>
-      </c>
-      <c r="M43" s="39" t="s">
-        <v>14</v>
-      </c>
-      <c r="N43" s="39" t="s">
-        <v>15</v>
-      </c>
-      <c r="O43" s="48">
-        <v>-1</v>
-      </c>
-      <c r="P43" s="48">
-        <v>874</v>
-      </c>
-      <c r="Q43" s="49">
-        <v>105612</v>
-      </c>
-      <c r="R43" s="39" t="s">
-        <v>47</v>
-      </c>
-      <c r="S43" s="39" t="s">
-        <v>31</v>
-      </c>
-      <c r="T43" s="47">
-        <v>26505</v>
-      </c>
-      <c r="U43" s="39" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="44" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="39" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="B44" s="39"/>
       <c r="C44" s="47" t="s">
         <v>78</v>
       </c>
       <c r="D44" s="39" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="E44" s="39"/>
       <c r="F44" s="39"/>
@@ -4206,13 +4225,13 @@
         <v>185</v>
       </c>
       <c r="J44" s="39" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="K44" s="39">
-        <v>-79.955122099999997</v>
+        <v>-79.956762600000005</v>
       </c>
       <c r="L44" s="39">
-        <v>39.669188599999998</v>
+        <v>39.637875299999997</v>
       </c>
       <c r="M44" s="39" t="s">
         <v>14</v>
@@ -4224,7 +4243,7 @@
         <v>-1</v>
       </c>
       <c r="P44" s="48">
-        <v>-1</v>
+        <v>874</v>
       </c>
       <c r="Q44" s="49">
         <v>105612</v>
@@ -4239,19 +4258,19 @@
         <v>26505</v>
       </c>
       <c r="U44" s="39" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="45" spans="1:21" s="42" customFormat="1" x14ac:dyDescent="0.2">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="45" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="39" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B45" s="39"/>
       <c r="C45" s="47" t="s">
         <v>78</v>
       </c>
       <c r="D45" s="39" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E45" s="39"/>
       <c r="F45" s="39"/>
@@ -4268,10 +4287,10 @@
         <v>181</v>
       </c>
       <c r="K45" s="39">
-        <v>-79.955245399999995</v>
+        <v>-79.955122099999997</v>
       </c>
       <c r="L45" s="39">
-        <v>39.669279500000002</v>
+        <v>39.669188599999998</v>
       </c>
       <c r="M45" s="39" t="s">
         <v>14</v>
@@ -4298,24 +4317,24 @@
         <v>26505</v>
       </c>
       <c r="U45" s="39" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="46" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="46" spans="1:21" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="39" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="B46" s="39"/>
       <c r="C46" s="47" t="s">
         <v>78</v>
       </c>
       <c r="D46" s="39" t="s">
-        <v>90</v>
+        <v>171</v>
       </c>
       <c r="E46" s="39"/>
       <c r="F46" s="39"/>
       <c r="G46" s="39" t="s">
-        <v>48</v>
+        <v>27</v>
       </c>
       <c r="H46" s="39" t="s">
         <v>76</v>
@@ -4324,13 +4343,13 @@
         <v>185</v>
       </c>
       <c r="J46" s="39" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="K46" s="39">
-        <v>-79.957359999999994</v>
+        <v>-79.955245399999995</v>
       </c>
       <c r="L46" s="39">
-        <v>39.625419999999998</v>
+        <v>39.669279500000002</v>
       </c>
       <c r="M46" s="39" t="s">
         <v>14</v>
@@ -4342,32 +4361,34 @@
         <v>-1</v>
       </c>
       <c r="P46" s="48">
-        <v>1851</v>
+        <v>-1</v>
       </c>
       <c r="Q46" s="49">
         <v>105612</v>
       </c>
       <c r="R46" s="39" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="S46" s="39" t="s">
         <v>31</v>
       </c>
       <c r="T46" s="47">
-        <v>26501</v>
-      </c>
-      <c r="U46" s="39"/>
+        <v>26505</v>
+      </c>
+      <c r="U46" s="39" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="47" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="39" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B47" s="39"/>
       <c r="C47" s="47" t="s">
         <v>78</v>
       </c>
       <c r="D47" s="39" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E47" s="39"/>
       <c r="F47" s="39"/>
@@ -4384,10 +4405,10 @@
         <v>180</v>
       </c>
       <c r="K47" s="39">
-        <v>-79.943309999999997</v>
+        <v>-79.957359999999994</v>
       </c>
       <c r="L47" s="39">
-        <v>39.61036</v>
+        <v>39.625419999999998</v>
       </c>
       <c r="M47" s="39" t="s">
         <v>14</v>
@@ -4399,7 +4420,7 @@
         <v>-1</v>
       </c>
       <c r="P47" s="48">
-        <v>726</v>
+        <v>1851</v>
       </c>
       <c r="Q47" s="49">
         <v>105612</v>
@@ -4417,19 +4438,19 @@
     </row>
     <row r="48" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A48" s="39" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="B48" s="39"/>
       <c r="C48" s="47" t="s">
         <v>78</v>
       </c>
       <c r="D48" s="39" t="s">
-        <v>233</v>
+        <v>92</v>
       </c>
       <c r="E48" s="39"/>
       <c r="F48" s="39"/>
       <c r="G48" s="39" t="s">
-        <v>27</v>
+        <v>48</v>
       </c>
       <c r="H48" s="39" t="s">
         <v>76</v>
@@ -4438,13 +4459,13 @@
         <v>185</v>
       </c>
       <c r="J48" s="39" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="K48" s="39">
-        <v>-79.965769100000003</v>
+        <v>-79.943309999999997</v>
       </c>
       <c r="L48" s="39">
-        <v>39.672765599999998</v>
+        <v>39.61036</v>
       </c>
       <c r="M48" s="39" t="s">
         <v>14</v>
@@ -4456,150 +4477,154 @@
         <v>-1</v>
       </c>
       <c r="P48" s="48">
-        <v>-1</v>
+        <v>726</v>
       </c>
       <c r="Q48" s="49">
         <v>105612</v>
       </c>
       <c r="R48" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="S48" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="T48" s="47">
+        <v>26501</v>
+      </c>
+      <c r="U48" s="39"/>
+    </row>
+    <row r="49" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="39" t="s">
+        <v>44</v>
+      </c>
+      <c r="B49" s="39"/>
+      <c r="C49" s="47" t="s">
+        <v>78</v>
+      </c>
+      <c r="D49" s="39" t="s">
+        <v>233</v>
+      </c>
+      <c r="E49" s="39"/>
+      <c r="F49" s="39"/>
+      <c r="G49" s="39" t="s">
+        <v>27</v>
+      </c>
+      <c r="H49" s="39" t="s">
+        <v>76</v>
+      </c>
+      <c r="I49" s="39" t="s">
+        <v>185</v>
+      </c>
+      <c r="J49" s="39" t="s">
+        <v>181</v>
+      </c>
+      <c r="K49" s="39">
+        <v>-79.965769100000003</v>
+      </c>
+      <c r="L49" s="39">
+        <v>39.672765599999998</v>
+      </c>
+      <c r="M49" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="N49" s="39" t="s">
+        <v>15</v>
+      </c>
+      <c r="O49" s="48">
+        <v>-1</v>
+      </c>
+      <c r="P49" s="48">
+        <v>-1</v>
+      </c>
+      <c r="Q49" s="49">
+        <v>105612</v>
+      </c>
+      <c r="R49" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="S48" s="39" t="s">
-        <v>31</v>
-      </c>
-      <c r="T48" s="47">
+      <c r="S49" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="T49" s="47">
         <v>26505</v>
       </c>
-      <c r="U48" s="39" t="s">
+      <c r="U49" s="39" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="49" spans="1:21" s="39" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="42" t="s">
+    <row r="50" spans="1:21" s="39" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="42" t="s">
         <v>199</v>
       </c>
-      <c r="B49" s="42"/>
-      <c r="C49" s="43" t="s">
+      <c r="B50" s="42"/>
+      <c r="C50" s="43" t="s">
         <v>78</v>
       </c>
-      <c r="D49" s="42" t="s">
+      <c r="D50" s="42" t="s">
         <v>200</v>
       </c>
-      <c r="E49" s="42"/>
-      <c r="F49" s="42">
+      <c r="E50" s="42"/>
+      <c r="F50" s="42">
         <v>54005012001</v>
       </c>
-      <c r="G49" s="42" t="s">
+      <c r="G50" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="H49" s="42" t="s">
+      <c r="H50" s="42" t="s">
         <v>76</v>
       </c>
-      <c r="I49" s="42" t="s">
-        <v>177</v>
-      </c>
-      <c r="J49" s="42" t="s">
-        <v>177</v>
-      </c>
-      <c r="K49" s="42">
+      <c r="I50" s="42" t="s">
+        <v>177</v>
+      </c>
+      <c r="J50" s="42" t="s">
+        <v>177</v>
+      </c>
+      <c r="K50" s="42">
         <v>-82.451303840583293</v>
       </c>
-      <c r="L49" s="42">
+      <c r="L50" s="42">
         <v>38.343336164586603</v>
       </c>
-      <c r="M49" s="42" t="s">
+      <c r="M50" s="42" t="s">
         <v>206</v>
       </c>
-      <c r="N49" s="42" t="s">
+      <c r="N50" s="42" t="s">
         <v>201</v>
       </c>
-      <c r="O49" s="52">
+      <c r="O50" s="52">
         <v>0.12</v>
       </c>
-      <c r="P49" s="52">
+      <c r="P50" s="52">
         <v>1600</v>
       </c>
-      <c r="Q49" s="50">
+      <c r="Q50" s="50">
         <v>42481</v>
       </c>
-      <c r="R49" s="53" t="s">
+      <c r="R50" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="S49" s="42" t="s">
-        <v>31</v>
-      </c>
-      <c r="T49" s="43">
+      <c r="S50" s="42" t="s">
+        <v>31</v>
+      </c>
+      <c r="T50" s="43">
         <v>25701</v>
       </c>
-      <c r="U49" s="42" t="s">
+      <c r="U50" s="42" t="s">
         <v>202</v>
-      </c>
-    </row>
-    <row r="50" spans="1:21" s="39" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="C50" s="47" t="s">
-        <v>78</v>
-      </c>
-      <c r="D50" s="39" t="s">
-        <v>93</v>
-      </c>
-      <c r="G50" s="39" t="s">
-        <v>48</v>
-      </c>
-      <c r="H50" s="39" t="s">
-        <v>76</v>
-      </c>
-      <c r="I50" s="39" t="s">
-        <v>185</v>
-      </c>
-      <c r="J50" s="39" t="s">
-        <v>180</v>
-      </c>
-      <c r="K50" s="39">
-        <v>-79.956739999999996</v>
-      </c>
-      <c r="L50" s="39">
-        <v>39.660640000000001</v>
-      </c>
-      <c r="M50" s="39" t="s">
-        <v>14</v>
-      </c>
-      <c r="N50" s="39" t="s">
-        <v>15</v>
-      </c>
-      <c r="O50" s="48">
-        <v>-1</v>
-      </c>
-      <c r="P50" s="48">
-        <v>688</v>
-      </c>
-      <c r="Q50" s="49">
-        <v>105612</v>
-      </c>
-      <c r="R50" s="39" t="s">
-        <v>55</v>
-      </c>
-      <c r="S50" s="39" t="s">
-        <v>31</v>
-      </c>
-      <c r="T50" s="47">
-        <v>26505</v>
       </c>
     </row>
     <row r="51" spans="1:21" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A51" s="39" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="C51" s="47" t="s">
         <v>78</v>
       </c>
       <c r="D51" s="39" t="s">
-        <v>164</v>
+        <v>93</v>
       </c>
       <c r="G51" s="39" t="s">
-        <v>26</v>
+        <v>48</v>
       </c>
       <c r="H51" s="39" t="s">
         <v>76</v>
@@ -4608,13 +4633,13 @@
         <v>185</v>
       </c>
       <c r="J51" s="39" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="K51" s="39">
-        <v>-79.953202899999994</v>
+        <v>-79.956739999999996</v>
       </c>
       <c r="L51" s="39">
-        <v>39.633116399999999</v>
+        <v>39.660640000000001</v>
       </c>
       <c r="M51" s="39" t="s">
         <v>14</v>
@@ -4626,13 +4651,13 @@
         <v>-1</v>
       </c>
       <c r="P51" s="48">
-        <v>-1</v>
+        <v>688</v>
       </c>
       <c r="Q51" s="49">
         <v>105612</v>
       </c>
       <c r="R51" s="39" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="S51" s="39" t="s">
         <v>31</v>
@@ -4640,22 +4665,19 @@
       <c r="T51" s="47">
         <v>26505</v>
       </c>
-      <c r="U51" s="39" t="s">
-        <v>160</v>
-      </c>
     </row>
     <row r="52" spans="1:21" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A52" s="39" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C52" s="47" t="s">
         <v>78</v>
       </c>
       <c r="D52" s="39" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G52" s="39" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H52" s="39" t="s">
         <v>76</v>
@@ -4664,13 +4686,13 @@
         <v>185</v>
       </c>
       <c r="J52" s="39" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="K52" s="39">
-        <v>-79.962211800000006</v>
+        <v>-79.953202899999994</v>
       </c>
       <c r="L52" s="39">
-        <v>39.6511596</v>
+        <v>39.633116399999999</v>
       </c>
       <c r="M52" s="39" t="s">
         <v>14</v>
@@ -4682,7 +4704,7 @@
         <v>-1</v>
       </c>
       <c r="P52" s="48">
-        <v>862</v>
+        <v>-1</v>
       </c>
       <c r="Q52" s="49">
         <v>105612</v>
@@ -4697,249 +4719,249 @@
         <v>26505</v>
       </c>
       <c r="U52" s="39" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="53" spans="1:21" s="39" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="C53" s="47" t="s">
+        <v>78</v>
+      </c>
+      <c r="D53" s="39" t="s">
+        <v>165</v>
+      </c>
+      <c r="G53" s="39" t="s">
+        <v>27</v>
+      </c>
+      <c r="H53" s="39" t="s">
+        <v>76</v>
+      </c>
+      <c r="I53" s="39" t="s">
+        <v>185</v>
+      </c>
+      <c r="J53" s="39" t="s">
+        <v>179</v>
+      </c>
+      <c r="K53" s="39">
+        <v>-79.962211800000006</v>
+      </c>
+      <c r="L53" s="39">
+        <v>39.6511596</v>
+      </c>
+      <c r="M53" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="N53" s="39" t="s">
+        <v>15</v>
+      </c>
+      <c r="O53" s="48">
+        <v>-1</v>
+      </c>
+      <c r="P53" s="48">
+        <v>862</v>
+      </c>
+      <c r="Q53" s="49">
+        <v>105612</v>
+      </c>
+      <c r="R53" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="S53" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="T53" s="47">
+        <v>26505</v>
+      </c>
+      <c r="U53" s="39" t="s">
         <v>157</v>
-      </c>
-    </row>
-    <row r="53" spans="1:21" s="39" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="42" t="s">
-        <v>230</v>
-      </c>
-      <c r="B53" s="42"/>
-      <c r="C53" s="43" t="s">
-        <v>78</v>
-      </c>
-      <c r="D53" s="42" t="s">
-        <v>231</v>
-      </c>
-      <c r="E53" s="42"/>
-      <c r="F53" s="42"/>
-      <c r="G53" s="42" t="s">
-        <v>27</v>
-      </c>
-      <c r="H53" s="42" t="s">
-        <v>76</v>
-      </c>
-      <c r="I53" s="42" t="s">
-        <v>185</v>
-      </c>
-      <c r="J53" s="42" t="s">
-        <v>179</v>
-      </c>
-      <c r="K53" s="42">
-        <v>-79.956140000000005</v>
-      </c>
-      <c r="L53" s="42">
-        <v>39.639200000000002</v>
-      </c>
-      <c r="M53" s="42" t="s">
-        <v>14</v>
-      </c>
-      <c r="N53" s="42" t="s">
-        <v>15</v>
-      </c>
-      <c r="O53" s="44">
-        <v>-1</v>
-      </c>
-      <c r="P53" s="44">
-        <v>474</v>
-      </c>
-      <c r="Q53" s="45">
-        <v>105612</v>
-      </c>
-      <c r="R53" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="S53" s="42" t="s">
-        <v>31</v>
-      </c>
-      <c r="T53" s="43">
-        <v>26505</v>
-      </c>
-      <c r="U53" s="42" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="54" spans="1:21" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A54" s="42" t="s">
-        <v>66</v>
-      </c>
-      <c r="B54" s="42" t="s">
-        <v>289</v>
-      </c>
+        <v>230</v>
+      </c>
+      <c r="B54" s="42"/>
       <c r="C54" s="43" t="s">
         <v>78</v>
       </c>
       <c r="D54" s="42" t="s">
+        <v>231</v>
+      </c>
+      <c r="E54" s="42"/>
+      <c r="F54" s="42"/>
+      <c r="G54" s="42" t="s">
+        <v>27</v>
+      </c>
+      <c r="H54" s="42" t="s">
+        <v>76</v>
+      </c>
+      <c r="I54" s="42" t="s">
+        <v>185</v>
+      </c>
+      <c r="J54" s="42" t="s">
+        <v>179</v>
+      </c>
+      <c r="K54" s="42">
+        <v>-79.956140000000005</v>
+      </c>
+      <c r="L54" s="42">
+        <v>39.639200000000002</v>
+      </c>
+      <c r="M54" s="42" t="s">
+        <v>14</v>
+      </c>
+      <c r="N54" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="O54" s="44">
+        <v>-1</v>
+      </c>
+      <c r="P54" s="44">
+        <v>474</v>
+      </c>
+      <c r="Q54" s="45">
+        <v>105612</v>
+      </c>
+      <c r="R54" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="S54" s="42" t="s">
+        <v>31</v>
+      </c>
+      <c r="T54" s="43">
+        <v>26505</v>
+      </c>
+      <c r="U54" s="42" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="55" spans="1:21" s="39" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="42" t="s">
+        <v>66</v>
+      </c>
+      <c r="B55" s="42" t="s">
+        <v>289</v>
+      </c>
+      <c r="C55" s="43" t="s">
+        <v>78</v>
+      </c>
+      <c r="D55" s="42" t="s">
         <v>97</v>
       </c>
-      <c r="E54" s="42">
+      <c r="E55" s="42">
         <v>-1</v>
       </c>
-      <c r="F54" s="42">
+      <c r="F55" s="42">
         <v>54003703001</v>
       </c>
-      <c r="G54" s="42" t="s">
+      <c r="G55" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="H54" s="42" t="s">
+      <c r="H55" s="42" t="s">
         <v>75</v>
       </c>
-      <c r="I54" s="42" t="s">
-        <v>177</v>
-      </c>
-      <c r="J54" s="42" t="s">
-        <v>177</v>
-      </c>
-      <c r="K54" s="42">
+      <c r="I55" s="42" t="s">
+        <v>177</v>
+      </c>
+      <c r="J55" s="42" t="s">
+        <v>177</v>
+      </c>
+      <c r="K55" s="42">
         <v>-81.205110000000005</v>
       </c>
-      <c r="L54" s="51">
+      <c r="L55" s="51">
         <v>39.391249999999999</v>
       </c>
-      <c r="M54" s="42" t="s">
+      <c r="M55" s="42" t="s">
         <v>66</v>
       </c>
-      <c r="N54" s="42" t="s">
+      <c r="N55" s="42" t="s">
         <v>71</v>
       </c>
-      <c r="O54" s="44">
+      <c r="O55" s="44">
         <v>0.52500000000000002</v>
       </c>
-      <c r="P54" s="45">
+      <c r="P55" s="45">
         <v>2892</v>
       </c>
-      <c r="Q54" s="45">
+      <c r="Q55" s="45">
         <v>7482</v>
       </c>
-      <c r="R54" s="46" t="s">
+      <c r="R55" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="S54" s="42" t="s">
-        <v>31</v>
-      </c>
-      <c r="T54" s="43">
+      <c r="S55" s="42" t="s">
+        <v>31</v>
+      </c>
+      <c r="T55" s="43">
         <v>26170</v>
       </c>
-      <c r="U54" s="42"/>
-    </row>
-    <row r="55" spans="1:21" s="39" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="39" t="s">
+      <c r="U55" s="42"/>
+    </row>
+    <row r="56" spans="1:21" s="39" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="39" t="s">
         <v>73</v>
       </c>
-      <c r="C55" s="47" t="s">
+      <c r="C56" s="47" t="s">
         <v>78</v>
       </c>
-      <c r="D55" s="39" t="s">
+      <c r="D56" s="39" t="s">
         <v>98</v>
       </c>
-      <c r="G55" s="39" t="s">
+      <c r="G56" s="39" t="s">
         <v>48</v>
       </c>
-      <c r="H55" s="39" t="s">
+      <c r="H56" s="39" t="s">
         <v>76</v>
       </c>
-      <c r="I55" s="39" t="s">
+      <c r="I56" s="39" t="s">
         <v>185</v>
       </c>
-      <c r="J55" s="39" t="s">
+      <c r="J56" s="39" t="s">
         <v>180</v>
       </c>
-      <c r="K55" s="39">
+      <c r="K56" s="39">
         <v>-79.978250000000003</v>
       </c>
-      <c r="L55" s="39">
+      <c r="L56" s="39">
         <v>39.671370000000003</v>
       </c>
-      <c r="M55" s="39" t="s">
+      <c r="M56" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="N55" s="39" t="s">
+      <c r="N56" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="O55" s="48">
+      <c r="O56" s="48">
         <v>-1</v>
       </c>
-      <c r="P55" s="48">
+      <c r="P56" s="48">
         <v>515</v>
       </c>
-      <c r="Q55" s="49">
+      <c r="Q56" s="49">
         <v>105612</v>
       </c>
-      <c r="R55" s="39" t="s">
+      <c r="R56" s="39" t="s">
         <v>55</v>
       </c>
-      <c r="S55" s="39" t="s">
-        <v>31</v>
-      </c>
-      <c r="T55" s="47">
+      <c r="S56" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="T56" s="47">
         <v>26505</v>
-      </c>
-    </row>
-    <row r="56" spans="1:21" s="42" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="42" t="s">
-        <v>36</v>
-      </c>
-      <c r="C56" s="43" t="s">
-        <v>78</v>
-      </c>
-      <c r="D56" s="42" t="s">
-        <v>172</v>
-      </c>
-      <c r="G56" s="42" t="s">
-        <v>27</v>
-      </c>
-      <c r="H56" s="42" t="s">
-        <v>76</v>
-      </c>
-      <c r="I56" s="42" t="s">
-        <v>185</v>
-      </c>
-      <c r="J56" s="42" t="s">
-        <v>179</v>
-      </c>
-      <c r="K56" s="42">
-        <v>-79.966336100000007</v>
-      </c>
-      <c r="L56" s="42">
-        <v>39.649548899999999</v>
-      </c>
-      <c r="M56" s="42" t="s">
-        <v>14</v>
-      </c>
-      <c r="N56" s="42" t="s">
-        <v>15</v>
-      </c>
-      <c r="O56" s="44">
-        <v>-1</v>
-      </c>
-      <c r="P56" s="44">
-        <v>904</v>
-      </c>
-      <c r="Q56" s="45">
-        <v>105612</v>
-      </c>
-      <c r="R56" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="S56" s="42" t="s">
-        <v>31</v>
-      </c>
-      <c r="T56" s="43">
-        <v>26505</v>
-      </c>
-      <c r="U56" s="42" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="57" spans="1:21" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A57" s="42" t="s">
-        <v>218</v>
+        <v>36</v>
       </c>
       <c r="C57" s="43" t="s">
         <v>78</v>
       </c>
       <c r="D57" s="42" t="s">
-        <v>219</v>
+        <v>172</v>
       </c>
       <c r="G57" s="42" t="s">
         <v>27</v>
@@ -4953,28 +4975,49 @@
       <c r="J57" s="42" t="s">
         <v>179</v>
       </c>
+      <c r="K57" s="42">
+        <v>-79.966336100000007</v>
+      </c>
+      <c r="L57" s="42">
+        <v>39.649548899999999</v>
+      </c>
+      <c r="M57" s="42" t="s">
+        <v>14</v>
+      </c>
       <c r="N57" s="42" t="s">
-        <v>191</v>
-      </c>
-      <c r="O57" s="44"/>
-      <c r="P57" s="44"/>
-      <c r="Q57" s="50">
-        <v>96319</v>
+        <v>15</v>
+      </c>
+      <c r="O57" s="44">
+        <v>-1</v>
+      </c>
+      <c r="P57" s="44">
+        <v>904</v>
+      </c>
+      <c r="Q57" s="45">
+        <v>105612</v>
+      </c>
+      <c r="R57" s="42" t="s">
+        <v>47</v>
       </c>
       <c r="S57" s="42" t="s">
         <v>31</v>
       </c>
-      <c r="T57" s="43"/>
+      <c r="T57" s="43">
+        <v>26505</v>
+      </c>
+      <c r="U57" s="42" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="58" spans="1:21" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A58" s="42" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C58" s="43" t="s">
         <v>78</v>
       </c>
       <c r="D58" s="42" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="G58" s="42" t="s">
         <v>27</v>
@@ -5002,370 +5045,348 @@
       <c r="T58" s="43"/>
     </row>
     <row r="59" spans="1:21" s="42" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="39" t="s">
+      <c r="A59" s="42" t="s">
+        <v>220</v>
+      </c>
+      <c r="C59" s="43" t="s">
+        <v>78</v>
+      </c>
+      <c r="D59" s="42" t="s">
+        <v>221</v>
+      </c>
+      <c r="G59" s="42" t="s">
+        <v>27</v>
+      </c>
+      <c r="H59" s="42" t="s">
+        <v>76</v>
+      </c>
+      <c r="I59" s="42" t="s">
+        <v>185</v>
+      </c>
+      <c r="J59" s="42" t="s">
+        <v>179</v>
+      </c>
+      <c r="N59" s="42" t="s">
+        <v>191</v>
+      </c>
+      <c r="O59" s="44"/>
+      <c r="P59" s="44"/>
+      <c r="Q59" s="50">
+        <v>96319</v>
+      </c>
+      <c r="S59" s="42" t="s">
+        <v>31</v>
+      </c>
+      <c r="T59" s="43"/>
+    </row>
+    <row r="60" spans="1:21" s="42" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="39" t="s">
         <v>51</v>
       </c>
-      <c r="B59" s="39"/>
-      <c r="C59" s="47" t="s">
+      <c r="B60" s="39"/>
+      <c r="C60" s="47" t="s">
         <v>78</v>
       </c>
-      <c r="D59" s="39" t="s">
+      <c r="D60" s="39" t="s">
         <v>99</v>
       </c>
-      <c r="E59" s="39"/>
-      <c r="F59" s="39"/>
-      <c r="G59" s="39" t="s">
+      <c r="E60" s="39"/>
+      <c r="F60" s="39"/>
+      <c r="G60" s="39" t="s">
         <v>48</v>
       </c>
-      <c r="H59" s="39" t="s">
+      <c r="H60" s="39" t="s">
         <v>76</v>
       </c>
-      <c r="I59" s="39" t="s">
+      <c r="I60" s="39" t="s">
         <v>185</v>
       </c>
-      <c r="J59" s="39" t="s">
+      <c r="J60" s="39" t="s">
         <v>180</v>
       </c>
-      <c r="K59" s="39">
+      <c r="K60" s="39">
         <v>-79.926150000000007</v>
       </c>
-      <c r="L59" s="39">
+      <c r="L60" s="39">
         <v>39.687820000000002</v>
       </c>
-      <c r="M59" s="39" t="s">
+      <c r="M60" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="N59" s="39" t="s">
+      <c r="N60" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="O59" s="48">
+      <c r="O60" s="48">
         <v>-1</v>
       </c>
-      <c r="P59" s="48">
+      <c r="P60" s="48">
         <v>1310</v>
       </c>
-      <c r="Q59" s="49">
+      <c r="Q60" s="49">
         <v>105612</v>
       </c>
-      <c r="R59" s="39" t="s">
+      <c r="R60" s="39" t="s">
         <v>55</v>
       </c>
-      <c r="S59" s="39" t="s">
-        <v>31</v>
-      </c>
-      <c r="T59" s="47">
+      <c r="S60" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="T60" s="47">
         <v>26508</v>
       </c>
-      <c r="U59" s="39"/>
-    </row>
-    <row r="60" spans="1:21" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="42" t="s">
-        <v>45</v>
-      </c>
-      <c r="C60" s="43" t="s">
-        <v>78</v>
-      </c>
-      <c r="D60" s="42" t="s">
-        <v>173</v>
-      </c>
-      <c r="G60" s="42" t="s">
-        <v>27</v>
-      </c>
-      <c r="H60" s="42" t="s">
-        <v>76</v>
-      </c>
-      <c r="I60" s="42" t="s">
-        <v>185</v>
-      </c>
-      <c r="J60" s="42" t="s">
-        <v>181</v>
-      </c>
-      <c r="K60" s="42">
-        <v>-79.956755900000005</v>
-      </c>
-      <c r="L60" s="42">
-        <v>39.640189999999997</v>
-      </c>
-      <c r="M60" s="42" t="s">
-        <v>14</v>
-      </c>
-      <c r="N60" s="42" t="s">
-        <v>15</v>
-      </c>
-      <c r="O60" s="44">
-        <v>-1</v>
-      </c>
-      <c r="P60" s="44">
-        <v>-1</v>
-      </c>
-      <c r="Q60" s="45">
-        <v>105612</v>
-      </c>
-      <c r="R60" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="S60" s="42" t="s">
-        <v>31</v>
-      </c>
-      <c r="T60" s="43">
-        <v>26505</v>
-      </c>
-      <c r="U60" s="42" t="s">
-        <v>62</v>
-      </c>
+      <c r="U60" s="39"/>
     </row>
     <row r="61" spans="1:21" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="42" t="s">
-        <v>12</v>
-      </c>
-      <c r="B61" s="42" t="s">
-        <v>291</v>
+        <v>45</v>
       </c>
       <c r="C61" s="43" t="s">
         <v>78</v>
       </c>
       <c r="D61" s="42" t="s">
-        <v>101</v>
-      </c>
-      <c r="E61" s="42" t="s">
-        <v>261</v>
-      </c>
-      <c r="F61" s="42">
-        <v>54002102001</v>
+        <v>173</v>
       </c>
       <c r="G61" s="42" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H61" s="42" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I61" s="42" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
       <c r="J61" s="42" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="K61" s="42">
-        <v>-80.459909999999994</v>
+        <v>-79.956755900000005</v>
       </c>
       <c r="L61" s="42">
-        <v>39.062240000000003</v>
+        <v>39.640189999999997</v>
       </c>
       <c r="M61" s="42" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="N61" s="42" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="O61" s="44">
-        <v>2.5</v>
-      </c>
-      <c r="P61" s="45">
-        <v>10364</v>
+        <v>-1</v>
+      </c>
+      <c r="P61" s="44">
+        <v>-1</v>
       </c>
       <c r="Q61" s="45">
-        <v>16166</v>
-      </c>
-      <c r="R61" s="46" t="s">
-        <v>18</v>
+        <v>105612</v>
+      </c>
+      <c r="R61" s="42" t="s">
+        <v>47</v>
       </c>
       <c r="S61" s="42" t="s">
         <v>31</v>
       </c>
       <c r="T61" s="43">
-        <v>26452</v>
+        <v>26505</v>
+      </c>
+      <c r="U61" s="42" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="62" spans="1:21" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="42" t="s">
-        <v>46</v>
+        <v>12</v>
+      </c>
+      <c r="B62" s="42" t="s">
+        <v>291</v>
       </c>
       <c r="C62" s="43" t="s">
         <v>78</v>
       </c>
       <c r="D62" s="42" t="s">
+        <v>101</v>
+      </c>
+      <c r="E62" s="42" t="s">
+        <v>261</v>
+      </c>
+      <c r="F62" s="42">
+        <v>54002102001</v>
+      </c>
+      <c r="G62" s="42" t="s">
+        <v>26</v>
+      </c>
+      <c r="H62" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="I62" s="42" t="s">
+        <v>177</v>
+      </c>
+      <c r="J62" s="42" t="s">
+        <v>177</v>
+      </c>
+      <c r="K62" s="42">
+        <v>-80.459909999999994</v>
+      </c>
+      <c r="L62" s="42">
+        <v>39.062240000000003</v>
+      </c>
+      <c r="M62" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="N62" s="42" t="s">
+        <v>13</v>
+      </c>
+      <c r="O62" s="44">
+        <v>2.5</v>
+      </c>
+      <c r="P62" s="45">
+        <v>10364</v>
+      </c>
+      <c r="Q62" s="45">
+        <v>16166</v>
+      </c>
+      <c r="R62" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="S62" s="42" t="s">
+        <v>31</v>
+      </c>
+      <c r="T62" s="43">
+        <v>26452</v>
+      </c>
+    </row>
+    <row r="63" spans="1:21" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="42" t="s">
+        <v>46</v>
+      </c>
+      <c r="C63" s="43" t="s">
+        <v>78</v>
+      </c>
+      <c r="D63" s="42" t="s">
         <v>174</v>
       </c>
-      <c r="G62" s="42" t="s">
+      <c r="G63" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="H62" s="42" t="s">
+      <c r="H63" s="42" t="s">
         <v>76</v>
       </c>
-      <c r="I62" s="42" t="s">
+      <c r="I63" s="42" t="s">
         <v>185</v>
       </c>
-      <c r="J62" s="42" t="s">
+      <c r="J63" s="42" t="s">
         <v>181</v>
       </c>
-      <c r="K62" s="42">
+      <c r="K63" s="42">
         <v>-79.925397000000004</v>
       </c>
-      <c r="L62" s="42">
+      <c r="L63" s="42">
         <v>39.6565887</v>
       </c>
-      <c r="M62" s="42" t="s">
+      <c r="M63" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="N62" s="42" t="s">
+      <c r="N63" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="O62" s="44">
+      <c r="O63" s="44">
         <v>-1</v>
       </c>
-      <c r="P62" s="44">
+      <c r="P63" s="44">
         <v>-1</v>
       </c>
-      <c r="Q62" s="45">
+      <c r="Q63" s="45">
         <v>105612</v>
       </c>
-      <c r="R62" s="42" t="s">
+      <c r="R63" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="S62" s="42" t="s">
-        <v>31</v>
-      </c>
-      <c r="T62" s="43">
+      <c r="S63" s="42" t="s">
+        <v>31</v>
+      </c>
+      <c r="T63" s="43">
         <v>26505</v>
       </c>
-      <c r="U62" s="42" t="s">
+      <c r="U63" s="42" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="63" spans="1:21" s="39" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="55" t="s">
+    <row r="64" spans="1:21" s="39" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="55" t="s">
         <v>23</v>
       </c>
-      <c r="B63" s="55" t="s">
+      <c r="B64" s="55" t="s">
         <v>265</v>
       </c>
-      <c r="C63" s="56" t="s">
+      <c r="C64" s="56" t="s">
         <v>224</v>
       </c>
-      <c r="D63" s="55" t="s">
+      <c r="D64" s="55" t="s">
         <v>83</v>
       </c>
-      <c r="E63" s="55" t="s">
+      <c r="E64" s="55" t="s">
         <v>260</v>
       </c>
-      <c r="F63" s="55">
+      <c r="F64" s="55">
         <v>54002701001</v>
       </c>
-      <c r="G63" s="55" t="s">
+      <c r="G64" s="55" t="s">
         <v>26</v>
       </c>
-      <c r="H63" s="55" t="s">
+      <c r="H64" s="55" t="s">
         <v>75</v>
       </c>
-      <c r="I63" s="55" t="s">
-        <v>177</v>
-      </c>
-      <c r="J63" s="55" t="s">
-        <v>177</v>
-      </c>
-      <c r="K63" s="55">
+      <c r="I64" s="55" t="s">
+        <v>177</v>
+      </c>
+      <c r="J64" s="55" t="s">
+        <v>177</v>
+      </c>
+      <c r="K64" s="55">
         <v>-81.015979999999999</v>
       </c>
-      <c r="L63" s="55">
+      <c r="L64" s="55">
         <v>37.42163</v>
       </c>
-      <c r="M63" s="55" t="s">
+      <c r="M64" s="55" t="s">
         <v>23</v>
       </c>
-      <c r="N63" s="55" t="s">
+      <c r="N64" s="55" t="s">
         <v>22</v>
       </c>
-      <c r="O63" s="58">
+      <c r="O64" s="58">
         <v>0.5</v>
       </c>
-      <c r="P63" s="59">
+      <c r="P64" s="59">
         <v>2391</v>
       </c>
-      <c r="Q63" s="59">
+      <c r="Q64" s="59">
         <v>58758</v>
       </c>
-      <c r="R63" s="60" t="s">
+      <c r="R64" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="S63" s="55" t="s">
-        <v>31</v>
-      </c>
-      <c r="T63" s="56">
+      <c r="S64" s="55" t="s">
+        <v>31</v>
+      </c>
+      <c r="T64" s="56">
         <v>24740</v>
       </c>
-      <c r="U63" s="55"/>
-    </row>
-    <row r="64" spans="1:21" s="39" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="19" t="s">
-        <v>132</v>
-      </c>
-      <c r="B64" s="19"/>
-      <c r="C64" s="20" t="s">
-        <v>224</v>
-      </c>
-      <c r="D64" s="19" t="s">
-        <v>139</v>
-      </c>
-      <c r="E64" s="19"/>
-      <c r="F64" s="41">
-        <v>54000101001</v>
-      </c>
-      <c r="G64" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="H64" s="19" t="s">
-        <v>75</v>
-      </c>
-      <c r="I64" s="19" t="s">
-        <v>177</v>
-      </c>
-      <c r="J64" s="19" t="s">
-        <v>177</v>
-      </c>
-      <c r="K64" s="19">
-        <v>-79.936940000000007</v>
-      </c>
-      <c r="L64" s="21">
-        <v>39.022010000000002</v>
-      </c>
-      <c r="M64" s="19" t="s">
-        <v>132</v>
-      </c>
-      <c r="N64" s="19" t="s">
-        <v>143</v>
-      </c>
-      <c r="O64" s="22">
-        <v>0.36499999999999999</v>
-      </c>
-      <c r="P64" s="23">
-        <v>1974</v>
-      </c>
-      <c r="Q64" s="23">
-        <v>16633</v>
-      </c>
-      <c r="R64" s="19"/>
-      <c r="S64" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="T64" s="20">
-        <v>26250</v>
-      </c>
-      <c r="U64" s="19"/>
+      <c r="U64" s="55"/>
     </row>
     <row r="65" spans="1:21" s="39" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="19" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B65" s="19"/>
       <c r="C65" s="20" t="s">
         <v>224</v>
       </c>
       <c r="D65" s="19" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="E65" s="19"/>
       <c r="F65" s="41">
-        <v>54003031001</v>
+        <v>54000101001</v>
       </c>
       <c r="G65" s="19" t="s">
         <v>26</v>
@@ -5380,49 +5401,49 @@
         <v>177</v>
       </c>
       <c r="K65" s="19">
-        <v>-80.212010000000006</v>
+        <v>-79.936940000000007</v>
       </c>
       <c r="L65" s="21">
-        <v>39.72007</v>
+        <v>39.022010000000002</v>
       </c>
       <c r="M65" s="19" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="N65" s="19" t="s">
-        <v>15</v>
+        <v>143</v>
       </c>
       <c r="O65" s="22">
-        <v>0.05</v>
-      </c>
-      <c r="P65" s="22">
-        <v>400</v>
+        <v>0.36499999999999999</v>
+      </c>
+      <c r="P65" s="23">
+        <v>1974</v>
       </c>
       <c r="Q65" s="23">
-        <v>105612</v>
+        <v>16633</v>
       </c>
       <c r="R65" s="19"/>
       <c r="S65" s="19" t="s">
         <v>31</v>
       </c>
       <c r="T65" s="20">
-        <v>26521</v>
+        <v>26250</v>
       </c>
       <c r="U65" s="19"/>
     </row>
     <row r="66" spans="1:21" s="39" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="19" t="s">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="B66" s="19"/>
       <c r="C66" s="20" t="s">
         <v>224</v>
       </c>
       <c r="D66" s="19" t="s">
-        <v>112</v>
+        <v>137</v>
       </c>
       <c r="E66" s="19"/>
       <c r="F66" s="41">
-        <v>54001702001</v>
+        <v>54003031001</v>
       </c>
       <c r="G66" s="19" t="s">
         <v>26</v>
@@ -5437,51 +5458,49 @@
         <v>177</v>
       </c>
       <c r="K66" s="19">
-        <v>-80.258989999999997</v>
+        <v>-80.212010000000006</v>
       </c>
       <c r="L66" s="21">
-        <v>39.280479999999997</v>
+        <v>39.72007</v>
       </c>
       <c r="M66" s="19" t="s">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="N66" s="19" t="s">
-        <v>106</v>
+        <v>15</v>
       </c>
       <c r="O66" s="22">
-        <v>3</v>
-      </c>
-      <c r="P66" s="23">
-        <v>6984</v>
+        <v>0.05</v>
+      </c>
+      <c r="P66" s="22">
+        <v>400</v>
       </c>
       <c r="Q66" s="23">
-        <v>67256</v>
-      </c>
-      <c r="R66" s="19" t="s">
-        <v>5</v>
-      </c>
+        <v>105612</v>
+      </c>
+      <c r="R66" s="19"/>
       <c r="S66" s="19" t="s">
         <v>31</v>
       </c>
       <c r="T66" s="20">
-        <v>26330</v>
+        <v>26521</v>
       </c>
       <c r="U66" s="19"/>
     </row>
     <row r="67" spans="1:21" s="39" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="19" t="s">
-        <v>68</v>
+        <v>110</v>
       </c>
       <c r="B67" s="19"/>
       <c r="C67" s="20" t="s">
         <v>224</v>
       </c>
       <c r="D67" s="19" t="s">
-        <v>85</v>
+        <v>112</v>
       </c>
       <c r="E67" s="19"/>
       <c r="F67" s="41">
-        <v>54002510001</v>
+        <v>54001702001</v>
       </c>
       <c r="G67" s="19" t="s">
         <v>26</v>
@@ -5496,51 +5515,51 @@
         <v>177</v>
       </c>
       <c r="K67" s="19">
-        <v>-80.567440000000005</v>
+        <v>-80.258989999999997</v>
       </c>
       <c r="L67" s="21">
-        <v>39.826610000000002</v>
+        <v>39.280479999999997</v>
       </c>
       <c r="M67" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="N67" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="O67" s="22">
+        <v>3</v>
+      </c>
+      <c r="P67" s="23">
+        <v>6984</v>
+      </c>
+      <c r="Q67" s="23">
+        <v>67256</v>
+      </c>
+      <c r="R67" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="S67" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="T67" s="20">
+        <v>26330</v>
+      </c>
+      <c r="U67" s="19"/>
+    </row>
+    <row r="68" spans="1:21" s="39" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="19" t="s">
         <v>68</v>
-      </c>
-      <c r="N67" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="O67" s="22">
-        <v>0.21</v>
-      </c>
-      <c r="P67" s="23">
-        <v>1340</v>
-      </c>
-      <c r="Q67" s="23">
-        <v>30531</v>
-      </c>
-      <c r="R67" s="37" t="s">
-        <v>18</v>
-      </c>
-      <c r="S67" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="T67" s="20">
-        <v>26033</v>
-      </c>
-      <c r="U67" s="19"/>
-    </row>
-    <row r="68" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="19" t="s">
-        <v>109</v>
       </c>
       <c r="B68" s="19"/>
       <c r="C68" s="20" t="s">
         <v>224</v>
       </c>
       <c r="D68" s="19" t="s">
-        <v>115</v>
+        <v>85</v>
       </c>
       <c r="E68" s="19"/>
       <c r="F68" s="41">
-        <v>54002405001</v>
+        <v>54002510001</v>
       </c>
       <c r="G68" s="19" t="s">
         <v>26</v>
@@ -5555,25 +5574,25 @@
         <v>177</v>
       </c>
       <c r="K68" s="19">
-        <v>-80.124449999999996</v>
+        <v>-80.567440000000005</v>
       </c>
       <c r="L68" s="21">
-        <v>39.493949999999998</v>
+        <v>39.826610000000002</v>
       </c>
       <c r="M68" s="19" t="s">
-        <v>109</v>
+        <v>68</v>
       </c>
       <c r="N68" s="19" t="s">
-        <v>107</v>
+        <v>9</v>
       </c>
       <c r="O68" s="22">
-        <v>9</v>
+        <v>0.21</v>
       </c>
       <c r="P68" s="23">
-        <v>25525</v>
+        <v>1340</v>
       </c>
       <c r="Q68" s="23">
-        <v>56072</v>
+        <v>30531</v>
       </c>
       <c r="R68" s="37" t="s">
         <v>18</v>
@@ -5582,258 +5601,264 @@
         <v>31</v>
       </c>
       <c r="T68" s="20">
+        <v>26033</v>
+      </c>
+      <c r="U68" s="19"/>
+    </row>
+    <row r="69" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="B69" s="19"/>
+      <c r="C69" s="20" t="s">
+        <v>224</v>
+      </c>
+      <c r="D69" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="E69" s="19"/>
+      <c r="F69" s="41">
+        <v>54002405001</v>
+      </c>
+      <c r="G69" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="H69" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="I69" s="19" t="s">
+        <v>177</v>
+      </c>
+      <c r="J69" s="19" t="s">
+        <v>177</v>
+      </c>
+      <c r="K69" s="19">
+        <v>-80.124449999999996</v>
+      </c>
+      <c r="L69" s="21">
+        <v>39.493949999999998</v>
+      </c>
+      <c r="M69" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="N69" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="O69" s="22">
+        <v>9</v>
+      </c>
+      <c r="P69" s="23">
+        <v>25525</v>
+      </c>
+      <c r="Q69" s="23">
+        <v>56072</v>
+      </c>
+      <c r="R69" s="37" t="s">
+        <v>18</v>
+      </c>
+      <c r="S69" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="T69" s="20">
         <v>26554</v>
       </c>
-      <c r="U68" s="19"/>
-    </row>
-    <row r="69" spans="1:21" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="55" t="s">
+      <c r="U69" s="19"/>
+    </row>
+    <row r="70" spans="1:21" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="55" t="s">
         <v>131</v>
       </c>
-      <c r="B69" s="55" t="s">
+      <c r="B70" s="55" t="s">
         <v>273</v>
       </c>
-      <c r="C69" s="56" t="s">
+      <c r="C70" s="56" t="s">
         <v>224</v>
       </c>
-      <c r="D69" s="55" t="s">
+      <c r="D70" s="55" t="s">
         <v>138</v>
       </c>
-      <c r="E69" s="55" t="s">
+      <c r="E70" s="55" t="s">
         <v>262</v>
       </c>
-      <c r="F69" s="55">
+      <c r="F70" s="55">
         <v>54000504001</v>
       </c>
-      <c r="G69" s="55" t="s">
+      <c r="G70" s="55" t="s">
         <v>26</v>
       </c>
-      <c r="H69" s="55" t="s">
+      <c r="H70" s="55" t="s">
         <v>75</v>
       </c>
-      <c r="I69" s="55" t="s">
-        <v>177</v>
-      </c>
-      <c r="J69" s="55" t="s">
-        <v>177</v>
-      </c>
-      <c r="K69" s="55">
+      <c r="I70" s="55" t="s">
+        <v>177</v>
+      </c>
+      <c r="J70" s="55" t="s">
+        <v>177</v>
+      </c>
+      <c r="K70" s="55">
         <v>-80.598290000000006</v>
       </c>
-      <c r="L69" s="57">
+      <c r="L70" s="57">
         <v>40.325800000000001</v>
       </c>
-      <c r="M69" s="55" t="s">
+      <c r="M70" s="55" t="s">
         <v>131</v>
       </c>
-      <c r="N69" s="55" t="s">
+      <c r="N70" s="55" t="s">
         <v>142</v>
       </c>
-      <c r="O69" s="58">
+      <c r="O70" s="58">
         <v>1.6</v>
       </c>
-      <c r="P69" s="59">
+      <c r="P70" s="59">
         <v>6468</v>
       </c>
-      <c r="Q69" s="59">
+      <c r="Q70" s="59">
         <v>21939</v>
       </c>
-      <c r="R69" s="60" t="s">
+      <c r="R70" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="S69" s="55" t="s">
-        <v>31</v>
-      </c>
-      <c r="T69" s="56">
+      <c r="S70" s="55" t="s">
+        <v>31</v>
+      </c>
+      <c r="T70" s="56">
         <v>26037</v>
       </c>
-      <c r="U69" s="55"/>
-    </row>
-    <row r="70" spans="1:21" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="B70" s="25"/>
-      <c r="C70" s="26" t="s">
-        <v>224</v>
-      </c>
-      <c r="D70" s="25" t="s">
-        <v>95</v>
-      </c>
-      <c r="E70" s="25">
-        <v>-1</v>
-      </c>
-      <c r="F70" s="25">
-        <v>54001205001</v>
-      </c>
-      <c r="G70" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="H70" s="25" t="s">
-        <v>75</v>
-      </c>
-      <c r="I70" s="25" t="s">
-        <v>177</v>
-      </c>
-      <c r="J70" s="25" t="s">
-        <v>177</v>
-      </c>
-      <c r="K70" s="25">
-        <v>-79.127250000000004</v>
-      </c>
-      <c r="L70" s="27">
-        <v>38.99091</v>
-      </c>
-      <c r="M70" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="N70" s="25" t="s">
-        <v>70</v>
-      </c>
-      <c r="O70" s="28">
-        <v>1.35</v>
-      </c>
-      <c r="P70" s="29">
-        <v>2700</v>
-      </c>
-      <c r="Q70" s="29">
-        <v>11616</v>
-      </c>
-      <c r="R70" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="S70" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="T70" s="26">
-        <v>26847</v>
-      </c>
-      <c r="U70" s="25"/>
+      <c r="U70" s="55"/>
     </row>
     <row r="71" spans="1:21" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="25" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="B71" s="25"/>
       <c r="C71" s="26" t="s">
         <v>224</v>
       </c>
       <c r="D71" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="E71" s="25">
+        <v>-1</v>
+      </c>
+      <c r="F71" s="25">
+        <v>54001205001</v>
+      </c>
+      <c r="G71" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="H71" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="I71" s="25" t="s">
+        <v>177</v>
+      </c>
+      <c r="J71" s="25" t="s">
+        <v>177</v>
+      </c>
+      <c r="K71" s="25">
+        <v>-79.127250000000004</v>
+      </c>
+      <c r="L71" s="27">
+        <v>38.99091</v>
+      </c>
+      <c r="M71" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="N71" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="O71" s="28">
+        <v>1.35</v>
+      </c>
+      <c r="P71" s="29">
+        <v>2700</v>
+      </c>
+      <c r="Q71" s="29">
+        <v>11616</v>
+      </c>
+      <c r="R71" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="S71" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="T71" s="26">
+        <v>26847</v>
+      </c>
+      <c r="U71" s="25"/>
+    </row>
+    <row r="72" spans="1:21" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="B72" s="25"/>
+      <c r="C72" s="26" t="s">
+        <v>224</v>
+      </c>
+      <c r="D72" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="E71" s="25"/>
-      <c r="F71" s="25"/>
-      <c r="G71" s="25" t="s">
+      <c r="E72" s="25"/>
+      <c r="F72" s="25"/>
+      <c r="G72" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="H71" s="25" t="s">
+      <c r="H72" s="25" t="s">
         <v>76</v>
       </c>
-      <c r="I71" s="4" t="s">
+      <c r="I72" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="J71" s="4" t="s">
+      <c r="J72" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="K71" s="25">
+      <c r="K72" s="25">
         <v>-78.98272</v>
       </c>
-      <c r="L71" s="27">
+      <c r="L72" s="27">
         <v>39.438070000000003</v>
       </c>
-      <c r="M71" s="25" t="s">
+      <c r="M72" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="N71" s="25" t="s">
+      <c r="N72" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="O71" s="28">
+      <c r="O72" s="28">
         <v>-1</v>
       </c>
-      <c r="P71" s="28">
+      <c r="P72" s="28">
         <v>1193</v>
       </c>
-      <c r="Q71" s="29">
+      <c r="Q72" s="29">
         <v>26868</v>
       </c>
-      <c r="R71" s="25" t="s">
+      <c r="R72" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="S71" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="T71" s="26">
+      <c r="S72" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="T72" s="26">
         <v>26726</v>
       </c>
-      <c r="U71" s="4"/>
-    </row>
-    <row r="72" spans="1:21" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="19" t="s">
-        <v>146</v>
-      </c>
-      <c r="B72" s="19"/>
-      <c r="C72" s="20" t="s">
-        <v>224</v>
-      </c>
-      <c r="D72" s="19" t="s">
-        <v>149</v>
-      </c>
-      <c r="E72" s="19"/>
-      <c r="F72" s="41">
-        <v>54004804001</v>
-      </c>
-      <c r="G72" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="H72" s="19" t="s">
-        <v>75</v>
-      </c>
-      <c r="I72" s="19" t="s">
-        <v>177</v>
-      </c>
-      <c r="J72" s="19" t="s">
-        <v>177</v>
-      </c>
-      <c r="K72" s="19"/>
-      <c r="L72" s="19"/>
-      <c r="M72" s="19" t="s">
-        <v>146</v>
-      </c>
-      <c r="N72" s="19" t="s">
-        <v>150</v>
-      </c>
-      <c r="O72" s="22">
-        <v>0.3</v>
-      </c>
-      <c r="P72" s="23">
-        <v>1800</v>
-      </c>
-      <c r="Q72" s="23">
-        <v>8811</v>
-      </c>
-      <c r="R72" s="19"/>
-      <c r="S72" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="T72" s="20"/>
-      <c r="U72"/>
+      <c r="U72" s="4"/>
     </row>
     <row r="73" spans="1:21" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="B73" t="s">
-        <v>290</v>
-      </c>
+        <v>146</v>
+      </c>
+      <c r="B73" s="19"/>
       <c r="C73" s="20" t="s">
         <v>224</v>
       </c>
       <c r="D73" s="19" t="s">
-        <v>100</v>
+        <v>149</v>
       </c>
       <c r="E73" s="19"/>
       <c r="F73" s="41">
-        <v>54003203001</v>
+        <v>54004804001</v>
       </c>
       <c r="G73" s="19" t="s">
         <v>26</v>
@@ -5847,52 +5872,46 @@
       <c r="J73" s="19" t="s">
         <v>177</v>
       </c>
-      <c r="K73" s="19">
-        <v>-78.226619999999997</v>
-      </c>
-      <c r="L73" s="19">
-        <v>39.628019999999999</v>
-      </c>
+      <c r="K73" s="19"/>
+      <c r="L73" s="19"/>
       <c r="M73" s="19" t="s">
-        <v>19</v>
+        <v>146</v>
       </c>
       <c r="N73" s="19" t="s">
-        <v>20</v>
+        <v>150</v>
       </c>
       <c r="O73" s="22">
-        <v>1.8</v>
+        <v>0.3</v>
       </c>
       <c r="P73" s="23">
-        <v>3255</v>
+        <v>1800</v>
       </c>
       <c r="Q73" s="23">
-        <v>17884</v>
-      </c>
-      <c r="R73" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="S73" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="T73" s="20">
-        <v>25411</v>
-      </c>
-      <c r="U73" s="19"/>
+        <v>8811</v>
+      </c>
+      <c r="R73" s="19"/>
+      <c r="S73" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="T73" s="20"/>
+      <c r="U73"/>
     </row>
     <row r="74" spans="1:21" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="19" t="s">
-        <v>147</v>
-      </c>
-      <c r="B74" s="19"/>
+        <v>19</v>
+      </c>
+      <c r="B74" t="s">
+        <v>290</v>
+      </c>
       <c r="C74" s="20" t="s">
         <v>224</v>
       </c>
       <c r="D74" s="19" t="s">
-        <v>148</v>
+        <v>100</v>
       </c>
       <c r="E74" s="19"/>
       <c r="F74" s="41">
-        <v>54000509001</v>
+        <v>54003203001</v>
       </c>
       <c r="G74" s="19" t="s">
         <v>26</v>
@@ -5906,44 +5925,52 @@
       <c r="J74" s="19" t="s">
         <v>177</v>
       </c>
-      <c r="K74" s="19"/>
-      <c r="L74" s="19"/>
+      <c r="K74" s="19">
+        <v>-78.226619999999997</v>
+      </c>
+      <c r="L74" s="19">
+        <v>39.628019999999999</v>
+      </c>
       <c r="M74" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="N74" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="O74" s="22">
+        <v>1.8</v>
+      </c>
+      <c r="P74" s="23">
+        <v>3255</v>
+      </c>
+      <c r="Q74" s="23">
+        <v>17884</v>
+      </c>
+      <c r="R74" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="S74" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="T74" s="20">
+        <v>25411</v>
+      </c>
+      <c r="U74" s="19"/>
+    </row>
+    <row r="75" spans="1:21" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="19" t="s">
         <v>147</v>
-      </c>
-      <c r="N74" s="19" t="s">
-        <v>142</v>
-      </c>
-      <c r="O74" s="22">
-        <v>4</v>
-      </c>
-      <c r="P74" s="23">
-        <v>20411</v>
-      </c>
-      <c r="Q74" s="15">
-        <v>21939</v>
-      </c>
-      <c r="R74" s="19"/>
-      <c r="S74" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="T74" s="20"/>
-      <c r="U74"/>
-    </row>
-    <row r="75" spans="1:21" s="42" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="19" t="s">
-        <v>108</v>
       </c>
       <c r="B75" s="19"/>
       <c r="C75" s="20" t="s">
         <v>224</v>
       </c>
       <c r="D75" s="19" t="s">
-        <v>114</v>
+        <v>148</v>
       </c>
       <c r="E75" s="19"/>
       <c r="F75" s="41">
-        <v>54002422001</v>
+        <v>54000509001</v>
       </c>
       <c r="G75" s="19" t="s">
         <v>26</v>
@@ -5957,42 +5984,93 @@
       <c r="J75" s="19" t="s">
         <v>177</v>
       </c>
-      <c r="K75" s="19">
+      <c r="K75" s="19"/>
+      <c r="L75" s="19"/>
+      <c r="M75" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="N75" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="O75" s="22">
+        <v>4</v>
+      </c>
+      <c r="P75" s="23">
+        <v>20411</v>
+      </c>
+      <c r="Q75" s="15">
+        <v>21939</v>
+      </c>
+      <c r="R75" s="19"/>
+      <c r="S75" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="T75" s="20"/>
+      <c r="U75"/>
+    </row>
+    <row r="76" spans="1:21" s="42" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="B76" s="19"/>
+      <c r="C76" s="20" t="s">
+        <v>224</v>
+      </c>
+      <c r="D76" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="E76" s="19"/>
+      <c r="F76" s="41">
+        <v>54002422001</v>
+      </c>
+      <c r="G76" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="H76" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="I76" s="19" t="s">
+        <v>177</v>
+      </c>
+      <c r="J76" s="19" t="s">
+        <v>177</v>
+      </c>
+      <c r="K76" s="19">
         <v>-80.260360000000006</v>
       </c>
-      <c r="L75" s="21">
+      <c r="L76" s="21">
         <v>39.452579999999998</v>
       </c>
-      <c r="M75" s="19" t="s">
+      <c r="M76" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="N75" s="19" t="s">
+      <c r="N76" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="O75" s="22">
+      <c r="O76" s="22">
         <v>0.1</v>
       </c>
-      <c r="P75" s="23">
+      <c r="P76" s="23">
         <v>2742</v>
       </c>
-      <c r="Q75" s="23">
+      <c r="Q76" s="23">
         <v>56072</v>
       </c>
-      <c r="R75" s="37" t="s">
+      <c r="R76" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="S75" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="T75" s="20">
+      <c r="S76" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="T76" s="20">
         <v>26591</v>
       </c>
-      <c r="U75" s="19"/>
+      <c r="U76" s="19"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:U77">
-    <sortCondition ref="C2:C77"/>
-    <sortCondition ref="A2:A77"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:U78">
+    <sortCondition ref="C2:C78"/>
+    <sortCondition ref="A2:A78"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated reports plus draft 1 of a sarvarDB summary script.
</commit_message>
<xml_diff>
--- a/analysis/resources/WaTCH_Tables.xlsx
+++ b/analysis/resources/WaTCH_Tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tpd0001/github/watch-wv/analysis/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5B2A7A9-9F6E-374A-A75A-7BCC59F97BB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90CA29AC-C0DC-7946-B174-5EF96A7741EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30040" windowHeight="14260" xr2:uid="{ABEE2980-A2EF-284E-9534-8BF6C1D1D8CC}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="911" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="955" uniqueCount="311">
   <si>
     <t>capacity_mgd</t>
   </si>
@@ -940,6 +940,33 @@
   </si>
   <si>
     <t>54019-001-01-00-00</t>
+  </si>
+  <si>
+    <t>StadiumSW-01</t>
+  </si>
+  <si>
+    <t>WVU Stadium SW</t>
+  </si>
+  <si>
+    <t>12-hr time-weighted composite</t>
+  </si>
+  <si>
+    <t>StadiumNW-01</t>
+  </si>
+  <si>
+    <t>StadiumNE-01</t>
+  </si>
+  <si>
+    <t>StadiumSE-01</t>
+  </si>
+  <si>
+    <t>WVU Stadium NW</t>
+  </si>
+  <si>
+    <t>WVU Stadium NE</t>
+  </si>
+  <si>
+    <t>WVU Stadium SE</t>
   </si>
 </sst>
 </file>
@@ -1582,13 +1609,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0856F7A-D0C0-3942-9027-9FB2F3C2C3E0}">
-  <dimension ref="A1:U76"/>
+  <dimension ref="A1:U80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B52" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B51" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B74" sqref="B74"/>
+      <selection pane="bottomRight" activeCell="G80" sqref="G80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6075,6 +6102,178 @@
       </c>
       <c r="U76" s="19"/>
     </row>
+    <row r="77" spans="1:21" s="39" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="39" t="s">
+        <v>302</v>
+      </c>
+      <c r="C77" s="47" t="s">
+        <v>122</v>
+      </c>
+      <c r="D77" s="39" t="s">
+        <v>303</v>
+      </c>
+      <c r="G77" s="42" t="s">
+        <v>26</v>
+      </c>
+      <c r="H77" s="39" t="s">
+        <v>76</v>
+      </c>
+      <c r="I77" s="39" t="s">
+        <v>185</v>
+      </c>
+      <c r="J77" s="39" t="s">
+        <v>184</v>
+      </c>
+      <c r="M77" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="N77" s="39" t="s">
+        <v>15</v>
+      </c>
+      <c r="O77" s="48"/>
+      <c r="P77" s="48"/>
+      <c r="Q77" s="49">
+        <v>105612</v>
+      </c>
+      <c r="R77" s="39" t="s">
+        <v>304</v>
+      </c>
+      <c r="S77" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="T77" s="47">
+        <v>26505</v>
+      </c>
+    </row>
+    <row r="78" spans="1:21" s="39" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A78" s="39" t="s">
+        <v>305</v>
+      </c>
+      <c r="C78" s="47" t="s">
+        <v>122</v>
+      </c>
+      <c r="D78" s="39" t="s">
+        <v>308</v>
+      </c>
+      <c r="G78" s="42" t="s">
+        <v>26</v>
+      </c>
+      <c r="H78" s="39" t="s">
+        <v>76</v>
+      </c>
+      <c r="I78" s="39" t="s">
+        <v>185</v>
+      </c>
+      <c r="J78" s="39" t="s">
+        <v>184</v>
+      </c>
+      <c r="M78" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="N78" s="39" t="s">
+        <v>15</v>
+      </c>
+      <c r="O78" s="48"/>
+      <c r="P78" s="48"/>
+      <c r="Q78" s="49">
+        <v>105612</v>
+      </c>
+      <c r="R78" s="39" t="s">
+        <v>304</v>
+      </c>
+      <c r="S78" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="T78" s="47">
+        <v>26505</v>
+      </c>
+    </row>
+    <row r="79" spans="1:21" s="39" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A79" s="39" t="s">
+        <v>306</v>
+      </c>
+      <c r="C79" s="47" t="s">
+        <v>122</v>
+      </c>
+      <c r="D79" s="39" t="s">
+        <v>309</v>
+      </c>
+      <c r="G79" s="42" t="s">
+        <v>26</v>
+      </c>
+      <c r="H79" s="39" t="s">
+        <v>76</v>
+      </c>
+      <c r="I79" s="39" t="s">
+        <v>185</v>
+      </c>
+      <c r="J79" s="39" t="s">
+        <v>184</v>
+      </c>
+      <c r="M79" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="N79" s="39" t="s">
+        <v>15</v>
+      </c>
+      <c r="O79" s="48"/>
+      <c r="P79" s="48"/>
+      <c r="Q79" s="49">
+        <v>105612</v>
+      </c>
+      <c r="R79" s="39" t="s">
+        <v>304</v>
+      </c>
+      <c r="S79" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="T79" s="47">
+        <v>26505</v>
+      </c>
+    </row>
+    <row r="80" spans="1:21" s="39" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A80" s="39" t="s">
+        <v>307</v>
+      </c>
+      <c r="C80" s="47" t="s">
+        <v>122</v>
+      </c>
+      <c r="D80" s="39" t="s">
+        <v>310</v>
+      </c>
+      <c r="G80" s="42" t="s">
+        <v>26</v>
+      </c>
+      <c r="H80" s="39" t="s">
+        <v>76</v>
+      </c>
+      <c r="I80" s="39" t="s">
+        <v>185</v>
+      </c>
+      <c r="J80" s="39" t="s">
+        <v>184</v>
+      </c>
+      <c r="M80" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="N80" s="39" t="s">
+        <v>15</v>
+      </c>
+      <c r="O80" s="48"/>
+      <c r="P80" s="48"/>
+      <c r="Q80" s="49">
+        <v>105612</v>
+      </c>
+      <c r="R80" s="39" t="s">
+        <v>304</v>
+      </c>
+      <c r="S80" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="T80" s="47">
+        <v>26505</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:U78">
     <sortCondition ref="C2:C78"/>

</xml_diff>

<commit_message>
Added WVU Coliseum to table of locations.
</commit_message>
<xml_diff>
--- a/analysis/resources/WaTCH_Tables.xlsx
+++ b/analysis/resources/WaTCH_Tables.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tpd0001/github/watch-wv/analysis/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90CA29AC-C0DC-7946-B174-5EF96A7741EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10F753B1-912F-9344-A595-E8C1DCF8B7D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30040" windowHeight="14260" xr2:uid="{ABEE2980-A2EF-284E-9534-8BF6C1D1D8CC}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="955" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="965" uniqueCount="313">
   <si>
     <t>capacity_mgd</t>
   </si>
@@ -967,6 +967,12 @@
   </si>
   <si>
     <t>WVU Stadium SE</t>
+  </si>
+  <si>
+    <t>Coliseum-01</t>
+  </si>
+  <si>
+    <t>WVU Coliseum</t>
   </si>
 </sst>
 </file>
@@ -1609,13 +1615,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0856F7A-D0C0-3942-9027-9FB2F3C2C3E0}">
-  <dimension ref="A1:U80"/>
+  <dimension ref="A1:U81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B51" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B57" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G80" sqref="G80"/>
+      <selection pane="bottomRight" activeCell="K80" sqref="K80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6274,6 +6280,50 @@
         <v>26505</v>
       </c>
     </row>
+    <row r="81" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A81" s="39" t="s">
+        <v>311</v>
+      </c>
+      <c r="C81" s="47" t="s">
+        <v>122</v>
+      </c>
+      <c r="D81" s="39" t="s">
+        <v>312</v>
+      </c>
+      <c r="G81" s="42" t="s">
+        <v>26</v>
+      </c>
+      <c r="H81" s="39" t="s">
+        <v>76</v>
+      </c>
+      <c r="I81" s="39" t="s">
+        <v>185</v>
+      </c>
+      <c r="J81" s="39" t="s">
+        <v>184</v>
+      </c>
+      <c r="K81">
+        <v>-79.985057699999999</v>
+      </c>
+      <c r="L81">
+        <v>39.648165400000003</v>
+      </c>
+      <c r="M81" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="N81" s="39" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q81" s="49">
+        <v>105612</v>
+      </c>
+      <c r="S81" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="T81" s="47">
+        <v>26505</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:U78">
     <sortCondition ref="C2:C78"/>

</xml_diff>